<commit_message>
was addited new articles 24/04
</commit_message>
<xml_diff>
--- a/BBC_reading/panddas.xlsx
+++ b/BBC_reading/panddas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="355">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -5641,6 +5641,1119 @@
   </si>
   <si>
     <t xml:space="preserve">Як багатії рятуються від коронавірусу. Огляд ЗМІ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 березня 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Посилений карантин у Британії: чого не можна робити – випуск новин 24.03.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">У випуску 24 березня:
+Чи запровадять в Україні надзвичайний стан?
+У Британії нові обмеження через пандемію.
+Переповнені лікарні в Іспанії: медики в розпачі.
+Антисептик від ПЦУ: як церква бореться з новим вірусом.
+Міфи про коронавірус: коров'яча сеча не захищає.
+Пропустити Youtube допис , автор: BBC News Україна
+Увага: інші сайти можуть містити рекламу
+Кінець Youtube допису , автор: BBC News Україна
+Ви також можете подивитись випуск на YouTube.
+Всі випуски новин на YouTube.
+І підписуйтеся на наш Youtube-канал!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Коронавірус в Україні. Інтерактивна мапа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В якій області найбільше інфікованих коронавірусом? Скільки одужало? А скільки померло? Все це - на нашій інтерактивній мапі.
+В Україні станом на 13:00 24 березня загалом зафіксували 97 випадків зараження коронавірусом. За минулу добу - 11 нових випадків, а за вівторок - 13 нових випадків, всі в Чернівецькій області.
+Усі дані про поширення коронавірусу в Україні - з інформаційних повідомлень міністерства охорони здоров'я, за винятком анексованого Росією Криму.
+Кількість підтверджених випадків зараження коронавірусом в Україні
+Джерело даних: МОЗ. *Дані по анексованому Криму взяті з російських офіційних джерел, перевірити їх у незалежних джерелах поки що неможливо. Підтверджених даних з ОРДЛО немає. Мапа створена за допомогою Carto.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Святослав Хоменко</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Як живе Київ на карантині</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+Тримільйонний Київ минулої п'ятниці оголосив режим надзвичайної ситуації. На той момент у місті вже закрили метро, торгові центри та ресторани.
+Київська влада закликала жителів міста залишатися вдома і не виходити на вулицю без крайньої потреби.
+До вівторка в Києві зафіксували 28 лабораторно підтверджених випадків захворювання на коронавірус.
+Від штрафів до в'язниці: як у світі запроваджують карантин
+Карантин: як пристосовується український бізнес
+Місяць без школи: як вчитися на карантині
+ВВС провела один день на вулицях Києва, щоб зрозуміти, як живе столиця України в обставинах надзвичайної ситуації, що змінюються мало не кожен день.
+Тролейбус за спецперепустками
+Спальний район Києва. На зупинці стоїть десяток людей, переважно літніх, у масках. Всі стоять ланцюжком: це черга на тролейбус. Люди хвилюються: у напівпорожній "шістнадцятий", який наближається до зупинки, швидше за все, потраплять не всі.
+Правила проїзду в міському транспорті Києва протягом останнього тижня неодноразово змінювалися.
+Спочатку закрили метро і обмежили кількість пасажирів міського транспорту до десяти людей на салон, причому обов'язково в масках. Обмеження, скажемо відверто, не працювало. Люди брали в облогу тролейбуси й автобуси, штовхалися з кондукторами, які намагалися просити вийти з салону зайвих пасажирів. Подекуди в ситуацію доводилося втручатися поліції.
+Image caption
+Так виглядають київські ринки
+Зрештою, на вихідних мер Києва Віталій Кличко анонсував чергове нововведення: громадський транспорт закривають для всіх, окрім власників спецперепусток.
+Картонні картки від мерії мали отримати тільки обрані: медпрацівники, правоохоронці, співробітники рятувальних служб, аптек, підприємств житлово-комунального господарства, а також продуктових магазинів. За перші кілька днів киянам видали понад двісті тисяч таких перепусток, а поліція відрапортувала, що знешкодила групу зловмисників, які намагалися продати фальшиві картки через інтернет.
+Але навіть наявність спецперепустки не гарантує його власникові місця у тролейбусі. "Шістнадцятий" зупиняється і через його передні двері виходять троє осіб. Водій голосно кричить: "Заходять троє, перепустку показуємо". Документи додатково перевіряє поліцейський, який сидить на передньому сидінні.
+Четвертою у черзі стоїть жінка у солідному респіраторі, вона в тролейбус не потрапляє.
+"Медпрацівнику можна, вашу мать?" - голосно обурюється вона. Водій розводить руками: правила є правила.
+Двері все ще напівпорожнього тролейбуса закриваються перед її носом, вона продовжує чортихатися.
+Штраф за дитячий майданчик
+У цій ситуації основним видом транспорту для багатьох киян стало таксі - ціни на його послуги залишилися на колишньому, докарантинному, рівні. Одразу кілька таксистів, з якими вдалося поговорити кореспондентам ВВС, стверджують: за останній тиждень роботи у них стало менше.
+Таксі возитиме лікарів безкоштовно через карантин
+"Клієнтів взагалі немає. До карантину як було: хто на роботу, хто з роботи, хто між офісами у справах, хто в аеропорт або на вокзал. Зараз всі або працюють віддалено, або взагалі з Києва повиїжджали", - каже Віталій, водій "Убера".
+І дійсно, вдень на вулицях Києва незвично мало людей. Майдан Незалежності порожній, тільки знімальна група якогось телеканалу записує стенд-ап кореспондента: кращого місця, щоб продемонструвати, що життя міста завмерло, й справді годі шукати.
+Однією з центральних вулиць повільно їде автомобіль рятувальної служби з мигалками й динаміками на даху. Суворий голос з колонок закликає киян залишатися вдома і обмежити до мінімуму кількість соціальних контактів.
+До останнього часу найжвавішими місцями у місті були парки й дитячі майданчики. Всі українські школи та дитсадки закрили на карантин ще з 12 березня, і батьки виводили дітей на свіже повітря, де ті раділи "коронтину, який від слова коронавірус".
+Але минулими вихідними Віталій Кличко наказав закрити усі дитячі майданчики міста, а порушників, які все ж виведуть дітей на гірки і гойдалки, пообіцяв штрафувати. Так само закрили й спортмайданчики.
+Вихідні в Києві видалися холодними і з мокрим снігом, тому в перший день розпорядження мера виконували на сто відсотків. Але у понеділок стало тепліше і обурених стало більше. Проте дитячі майданчики вже були обнесені червоно-білими стрічками і обклеєні оголошеннями про заборону. У соцмережах і батьківських групах з'явилися критичні коментарі: діти в чотири стінах, мовляв, виносять мозок.
+"Не вигуляні діти - це точно краще, ніж мертва бабуся", - оцінив такі коментарі у себе у Facebook київський публіцист Дмитро Литвин.
+"Масок немає"
+Ще минулого тижня у Києві закрили всі кафе, ресторани, торгові центри, спортзали і магазини, окрім продуктових. Працюють також аптеки і частина банківських відділень.
+На деяких закритих манікюрних салонах і перукарнях можна побачити записки з текстом на кшталт "З будь-яких питань звертайтесь за телефоном", або простіше - "Стрижка на дому".
+Втім, велика частина бізнесів, які закрилися - від ресторанів до секс-шопів - перейшли на обслуговування клієнтів онлайн з доставкою замовлених страв і товарів додому.
+А перед "офлайновими" супермаркетами шикуються черги. Київська мерія визначила, що усі торгові точки міста мають право запускати по одній людині на десять квадратних метрів своєї площі, тому бажаючі купити продукти можуть увійти до магазину тільки після того, як звідти вийде попередній клієнт.
+У перші дні обмежень у великих супермаркетах на касах шикувалися черги по кілька десятків людей: люди розбирали крупи, макарони, сіль, консерви. Однак вже за кілька днів паніка зникла.
+Деякі магазини не пускають всередину клієнтів без масок, хоча б і саморобних, зроблених з марлі, поролону або навіть паперового рушника. Інші - закривають на це очі.
+Як коронавірус шириться планетою. Мапа
+Коронавірус: що треба знати
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Такі ж черги стоять перед розкиданими по всьому Києву відділеннями найпопулярнішої служби доставки "Нова пошта": через інтернет сюди можна замовити хоч ящик вина, хоч холодильник.
+Так само люди стоять перед аптеками. На дверях чи не кожної - найчастіше написана від руки записка: "Масок немає".
+На одній аптеці такого папірця немає. Звертаюся до жінки за стійкою: "Маски ..." Вона не дає закінчити: "Маски, рукавички, спирт, антисептики, гліцерин, перекис, парацетамол". Питаю: "Усе є?" Вона посміхається: "Усього немає. Питання до постачальника. Вранці повинні були підвезти, але не підвезли".
+Втім, якщо дійсно поставити собі за мету знайти флакон перекису водню або пляшечку хлоргексидину, то це можливо. Головне - не втрачати надії. І стояти хвилин по п'ять у черзі перед кожною аптекою.
+Копирайт изображения
+GETTY IMAGES
+З масками складніше - в аптеках їх дійсно немає. Зате у Facebook та Instagram з'явилася контекстна реклама крафтових масок або "масок з логотипом вашої фірми". Напередодні Православна церква Московського патріархату заявила, що кравецькі майстерні Києво-Печерської лаври переорієнтуються на виробництво захисних масок. А священники відділу соціального служіння Православної церкви України у київському Видубицькому монастирі виготовляють антисептики.
+"До останнього клієнта"
+Карантин помітно позначився на житті спальних районів Києва. Закрилася частина маленьких кав'ярень, які складають значну частину київського міського пейзажу. Ті, що не зачинилися, обслуговують клієнтів біля дверей: продають каву з собою.
+Продовжили працювати кіоски з мобільними телефонами і аксесуарами: їм продавці демонструють постанову уряду, що дозволяє роботу торгових точок, які реалізовують засоби зв'язку. Так само продовжують працювати ломбарди.
+Як не дивно, відкритими залишилися і магазини, які торгують розливним пивом і вином. Заходжу в одну з таких торгових точок і знайомлюся з нудьгуючим молодим хлопцем Артемом (ім'я змінено).
+Питаю у нього: "Як іде торгівля?"
+"Якщо я вам скажу, що добре, і ось так посміхнусь, ви мені повірите?" - відповідає Артем і робить такий вираз обличчя, що стає зрозуміло: його магазин на межі банкрутства.
+"Ми теж думали, що нам зараз попре, але щось пішло не так", - пояснює він.
+Обійти обмеження на роботу торгових точок його магазину вдалося просто. Артем звертає мою увагу на невеликий ящик в кутку магазину. У ньому складені кілька банок курячого паштету, дві пачки макаронів, банка оливок і консервованих томатів. З таким асортиментом його наливайка цілком може називатися продуктовим магазином, робота яких у Києві має тривати попри карантин.
+"Скажу вам так: ми - як друга аптека. Повинен же хтось людей рятувати. У цих, - Артем невизначено махає рукою, - не виходить. А це значить, ми будемо працювати до останнього клієнта".
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Антисептик від ПЦУ: як церква бореться з коронавірусом</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Надзвичайний стан Авакова: як зростає роль міністра внутрішніх справ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+УНІАН
+У першому уряді за президента Зеленського керівника МВС Арсена Авакова називали "тимчасовим міністром", який пропрацює кілька місяців.
+Утім, тимчасовим виявився Кабмін Гончарука, тоді як Аваков залишився працювати в новому уряді Шмигаля і відзначив шість років на посаді міністра внутрішніх справ.
+Надзвичайний стан. Що це означає і які можуть бути обмеження
+Як коронавірус шириться планетою. Мапа
+Зараз його вже не називають "тимчасовим", він керує найпотужнішою структурою в умовах карантину і радить Верховній Раді та всьому уряду, що треба зробити в економіці.
+А також - готує суспільство до введення надзвичайного стану, який ще більше розширить повноваження його міністерства.
+Силовики і карантин
+Арсена Авакова називали однією з проблем формування уряду Дениса Шмигаля. Через це, зокрема, за новий Кабмін голосували пакетом, адже не факт, що при поіменному голосуванні за кожного з міністрів знайшлося б достатньо голосів.
+Утім, з початком спалаху коронавірусу в Україні керівник МВС став однією з ключових фігур не тільки в Кабміні, але й у державі загалом.
+Поліція та інші підрозділи, які входять до структури міністерства внутрішніх справ - Нацгвардія, Держслужба з надзвичайних ситуацій і Прикордонна служба - зараз мають головну роль у всіх карантинних заходах.
+Відділення спецобробки ДСНС проводить знезараження у Радомишлі, де був один з перших підтверджених випадків коронавірусу в країні, авіація Нацгвардії доправляє з Китаю тести та костюми хімзахисту, а поліцейсьі у великих містах стежать, кого і скільки перевозить громадський транспорт.
+З подачі МВС посилена відповідальність за порушення карантину — за це тепер штрафи від 17 до 32 тис. грн.
+Крім того, за навмисне зараження коронавірусом інших людей можна потрапити до в'язниці на строк до восьми років. У МВС пояснюють, що в'язниця загрожуватиме лише тим, хто точно знав про свою хворобу і свідомо заражав нею інших, наприклад, у транспорті.
+На пів дорозі до надзвичайного стану?
+МВС стало локомотивом введення надзвичайної ситуації в областях, де виявили коронавірус.
+За Кодексом цивільного захисту населення - це етап, який може передувати надзвичайному стану.
+Арсен Аваков нещодавно написав, що у найближчі дні обмеження "будуть значно жорсткішими".
+За його словами, це потрібно, щоб виграти час для системи охорони здоров'я: "Кожен день не надмірної напруги нашої перехідної, кульгавої медичної системи — важливий!"
+Пропустити Facebook допис , автор: Arsen
+Дорогие украинцы! События последних дней кардинально изменили жизнь всего общества и всего мира. Мир меняется и...
+Posted by Arsen Avakov on Saturday, 21 March 2020
+Кінець Facebook допису , автор: Arsen
+Про те, що вже введені обмеження недостатні, говорять й інші люди з команди Авакова.
+"Все буде залежати від статистики, зокрема смертності... Попереду у нас буде піт, кров і сльози, як казав прем'єр-міністр Британії Вінстон Черчилль перед Другою світовою війною", - заявив у "Свободі слова" на ICTV заступник міністра внутрішніх справ Антон Геращенко.
+Він також порівняв нинішній спалах коронавірусу з епідемією "іспанки" у 1918-1919 роках, від якої загинули кілька десятків мільйонів людей.
+Антон Герщенко попередив тих, хто вже міг заразитися (наприклад, повернувся з-за кордону), що вони мають дотримуватися самоізоляції.
+"Поліція почала централізовано отримувати контакти з ваших анкет. За необхідності будемо звертатися до мобільних операторів, будемо звертатися до банківської сфери. Ви зобов'язані перебувати вдома, щоб зберегти життя своїх близьких", - закликав заступник міністра.
+І додав: "У нас карантин зараз на 50-60%. В Італії та Іспанії — на 95%... Ми до цього часу зупинилися на пів дорозі. І продовжується величезне спілкування людей з людьми".
+За даними BBC News Україна, Верховна Рада може винести на голосування надзвичайний стан вже цього тижня.
+Він - значно суворіший за нинішні надзвичайні ситуації і може передбачати серйозні обмеження, аж до блокпостів і заборони руху на особистому транспорті між містами. Видання Insider також писало про плани запровадити можливість комендантської години та обшуків під час пандемії.
+Контролюватимуть дотримання надзвичайного стану, якщо його коли-небудь все ж запровадять, саме структури МВС.
+Водночас у вівторок ввечері Арсен Аваков у коментарі "Українській правді" запевнив, що наразі не бачить сенсу у запровадженні надзвичайного стану.
+"Для забезпечення карантину нам цілком досить оголошення режиму надзвичайної ситуації, який зараз діє в Києві і інших містах… Надзвичайний стан зараз не потрібен. Він передбачає обмеження конституційних прав. Для боротьби з вірусом нам це ні до чого. Його запровадження може бути тільки крайнім заходом", - пояснив міністр.
+А що з економікою?
+Паралельно Арсен Аваков почав давати поради уряду та парламенту у сферах, які виходять за межі його компетенції як міністра внутрішніх справ - в економіці та фінансах.
+Він закликав переглянути Держбюджет, значно збільшити його дефіцит, укласти угоду з МВФ та реструктуризувати зовнішні борги, щоб менше виплачувати у найближчі роки.
+"Без цих та інших екстраординарних заходів буде жахливо складно! Людям буде дуже складно! І тому треба діяти, захищаючи людей, балансуючи економіку в умовах, яких ще не було", - наголосив Аваков.
+"Вимушена необхідність"
+"Посилення ролі Арсена Авакова у часи кризи, пов'язаної з пандемією, я називаю "вимушеною необхідністю". В умовах, коли урядовці не знають, що робити з кризою, активність Авакова я вважаю позитивом", - говорить BBC News Україна політичний консультант Петро Охотін.
+Петро Охотін додає, що МВС ще з часів Леоніда Кучми має чи не найбільш чітку і дієву вертикаль серед усіх інших державних інститутів.
+"Роль Арсена Авакова зростає в умовах, коли інші чиновники намагаються взяти на себе якомога менше відповідальності, адже Кабмін Дениса Шмигаля формувався не як антикризовий, а радше як консенсусний", - відзначає політичний консультант.
+"З одного боку, фігура Авакова не раз піддавалася критиці. З іншого, просто уявіть, що Арсен Борисович зараз вирішить піти у відставку. Очевидно, що слабкість державної вертикалі і некомпетентність команди Зеленського створює всі умови для приходу сил, готових до більш авторитарних дій. Ще давні греки казали: "анархія - мати порядку", адже після хаосу часто встановлювалися тиранії", - вважає Петро Охотін.
+Новий фаворит
+Керівник аналітичної групи "Левіафан" Микола Мельник каже, що політична вага Арсена Авакова поступово зростала протягом президентства Зеленського.
+"Роль Авакова аномально зросла не сьогодні, це був доволі тривалий процес, що розпочався з моменту формування коаліційного уряду Гончарука. А потім комом зростав до пресконференції щодо "призначення" винних у справі Шеремета", - пригадує аналітик.
+У МВС наполягають, що не "призначали" нікого винним у цій справі, а лише говорили про людей, які "обгрунтовано підозрюються" у причетності до вбивства журналіста. Тим не менше, згадана пресконференція, ще й за участі глави держави, викликала значний резонанс та критику через наведені докази, які захист затриманих вважає сумнівними.
+Поліція затримала підозрюваних у справі Шеремета. Серед них музикант Riffmaster?
+"Потім роль Авакова у державницьких процесах лише зростала, адже слід пам'ятати, що Аваков - це не тільки МВС, це і Мінінфраструктури та пару десятків депутатів у парламенті", - додає Микола Мельник.
+На його думку, роль Арсена Авакова буде зростати, поки Володимир Зеленський "буде вбачати в українцях, які його не підтримують, загрозу".
+"А картинка для цього створюється ідеальна. Це і "падіння Сивохи", і "бійки за землю" на Грушевського, і заяви волонтерки" Звіробій та депутатки Федини", - додає аналітик.
+На його думку, найбільше сила Авакова зросте якраз із введенням надзвичайного стану: "Адже саме на нього буде покладене його дотримання".
+"Він суто психологічно сильніший за всіх в оточенні президента і вміє переконувати Зеленського в своїй правоті. Чим, до речі, можуть похвалитись одиниці", - відзначає Мельник.
+За його словами, Аваков вже вписався у схему "фаворитів" Зеленського, яку раніше очолював Андрій Богдан і яка існує через "вакуум влади" навколо президента.
+"Можливо, цей вакуум виникає через те, що Зеленський щиро намагається побудувати систему управління шляхом корпоративного делегування повноважень. А в умовах української традиції держуправління це сприймається як слабкість. Кожен намагається цей вакуум заповнити", - резюмує Микола Мельник.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Євгенія Ковалевська</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тести на коронавірус: скільки їх треба Україні</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+AFP
+Image caption
+У ВООЗ закликають країни до інтенсивного тестування
+Вночі з українського військового літака, що прилетів з Китаю, вивантажують коробки. Весь процес уважно фотографують і знімають.
+Президент записує відеозвернення, МОЗ звітує - 250 тисяч експрес-тестів, а також тестів ПЛР нарешті приїхали до України.
+"Тестувати, тестувати і тестувати. Всі підозрілі випадки", - закликав доктор Тедрос Аданом Гебрейесус, генеральний директор ВООЗ.
+Поки в Південній Кореї, наприклад, протестували 290 тисяч людей, а у Британії понад 40 тисяч, в Україні лише 850 людей.
+Коронавірус у Південній Кореї йде на спад: як їм це вдалося?
+Pornhub дає безкоштовну преміум-підписку всім. На час карантину
+Чи вистачить Україні 250 тисяч тестів для того, аби виявити коронавірус і зупинити його поширення? Чому в країні так мало протестованих людей?
+І чи варто госпіталізовувати тих, у кого підтвердили covid-19?
+В Україну привезли сотні тисяч тестів на коронавірус. Кому їх передадуть?
+Як зробити тест на коронавірус? Питання і відповіді
+Кількість формує потребу
+В Офісі президента запевняють, що отримані тести - лише перша партія медичного вантажу, всього їх буде декілька і вже цього тижня.
+За словами Володимира Зеленського, Україна загалом розраховує отримати 10 млн тестів.
+У Центрі громадського здоров'я розповіли, що вони отримали 521 тест-систему полімеразної ланцюгової реакції (ПЛР).
+Їхня потужність - 50 тисяч реакцій, тобто можна протестувати до 50 тисяч людей.
+Копирайт изображения
+FACEBOOK.COM/KIRILL.TIMOSHENKO
+Image caption
+З Кита до України приїхали тести
+Як повідомив заступник міністра охорони здоров'я Віктор Ляшко, тести ПЛР роблять у 25 лабораторіях в Україні. Це займає всього кілька годин.
+Отримані тести розподілять між регіонами пропорційно до кількості населення.
+Вже у вівторок, 24 березня, вони мають бути у всіх областях.
+"Кількість тестів формується від потреби. Ми дивимося, як розвиватиметься ситуація", - повідомили ВВС News Україна в пресслужбі МОЗ.
+Кого треба тестувати
+Вірусолог Алла Мироненко вважає, що 50 тисяч досліджень, які можуть провести за допомогою ПЛР, це багато.
+"На період епідемії цього точно вистачить. А тестування на місці, в регіональних лабораторіях, буде більш точним і прицільним, і, звісно, швидшим", - додає пані Мироненко, яка працює в Інституті епідеміології та інфекційних хвороб.
+Вона підраховує, що кожна область зможе зробити близько двох тисяч досліджень на коронавірус.
+"Якщо в регіоні вже є епідемічна ситуація і наявна типова клінічна картина, то чи треба обстежувати всіх? На початку - треба, для підтвердження важких випадків - треба. А так, може, і не треба - є симптоматика, є алгоритм лікування", - додає вірусолог.
+За її словами, легкі форми захворювання можна лікувати, не підтверджуючи тестом. Адже якихось особливих ліків проти коронавірусу не існує.
+Копирайт изображения
+FACEBOOK.COM/KIRILL.TIMOSHENKO
+Експертка додала, що психологічна напруга і карантин іноді викликають у людей нав'язливі думки про хворобу.
+"Багато людей перебувають в такому психологічному стані, що їм здається, що саме в них утруднене дихання. Вони приходять на прийом і настирливо вимагають у лікаря госпіталізації", - додала Алла Мироненко.
+Чому протестували так мало людей
+За повідомленням Центру громадського здоров'я, станом на понеділок, 23 березня, в Україні протестували близько 850 людей.
+Ці дані не є показником для всієї території України, тому що є ще регіональні та приватні лабораторії.
+Загальної статистики не ведуть. Лабораторії повідомляють про підтверджені випадки, пояснили в Центрі.
+Для порівняння, у Південній Кореї тести на коронавірус зробили 290 тисячам людей, у Великій Британії понад 40 тисячам, у Білорусі - 16 тисячам. То чому в Україні протестували так мало людей і чи має ця цифра бути більшою?
+У Міністерстві охорони здоров'я кажуть, що раніше пацієнту робили тест на грип, коли результат був негативний, робили експрес-тест на коронавірус.
+Тепер, коли в Україну прибула перша велика партія тестів, за наявності ознак хвороби одразу робитимуть експрес-тест на коронавірус.
+Тому можна очікувати зростання кількості протестованих.
+Як повернутися в Україну: що радять українцям, які застрягли за кордоном через коронавірус
+Які прикордонні пункти закривають через коронавірус. Повний список
+"Ніхто не знає, що буде завтра". Що кажуть про карантин українці в Італії
+Масштабне тестування важливе…
+В Україні треба протестувати значно більшу кількість людей, ніж є зараз, переконана голова Представництва ЮНІСЕФ в Україні Лотта Сильвандер.
+"Якщо подивимося на країни, яким вдалося знизити рівень захворюваності на коронавірус, то побачимо, що вони проводили масштабне тестування населення і точно визначали коло осіб, які контактували з інфікованим", - розповідає пані Сильвандер.
+Водночас, за словами очільниці з ЮНІСЕФ, для України, окрім кількості тестів, важливими також є два інші моменти: компетенція і безпека медиків та достатня кількість лабораторій з відповідним обладнанням.
+Копирайт изображения
+CITY-ADM.LVIV.UA
+Image caption
+Експрес-тести на коронавірус виглядають так
+"Зараз Україна не має можливості робити велику кількість тестів. В країні немає достатньо захисних костюмів для лікарів та недостатня спроможність лабораторій проводити велику кількість тестів одночасно, навіть якщо тест-системи з'являться".
+Пані Сильвандер наголошує: яким би не був результат експрес-тесту, його треба підтвердити тестом ПЛР.
+Для експрес-тесту беруть мазок з носа, й результат готовий за 15 хвилин. Перевірку методом ПЛР роблять лише у спеціальних лабораторіях.
+…але це ще не все
+Інший незрозумілий момент в Україні, зазначає голова Представництва ЮНІСЕФ, - що ж робити, якщо у пацієнта підтвердили коронавірус.
+"Якщо за результатами тесту у людини підтвердили коронавірус, це не означає, що вона має бути госпіталізована чи отримувати лікування. Багато пацієнтів з covid-19 не потребують цього всього. Вони залишаються вдома в самоізоляції", - описує світовий досвід Лотта Сильвандер.
+За її словами, в Україні немає чіткості у підходах, що робити з пацієнтом, у якого підтвердили коронавірус.
+Пропустити Youtube допис , автор: BBC News Україна
+Увага: інші сайти можуть містити рекламу
+Кінець Youtube допису , автор: BBC News Україна
+А що з лабораторіями і лікарями?
+Те, що обмежена кількість тестів - не єдина проблема в Україні, переконаний і Павло Ковтонюк, заступник міністра охорони здоров'я у 2016-2019 роках.
+"Тестів більш-менш достатньо. До кінця карантину можна буде широко тестувати", - каже він.
+Але є проблема з потужністю лабораторій, які будуть робити тести, і в системі виявлення. "Хтось же повинен цю людину знайти, направити і протестувати. Ці дві речі зараз сильно відстають", - пояснює експерт.
+За його словами, державних лабораторій в Україні небагато і їхня максимальна потужність - до тисячі тестів в день.
+"Щоб я робив - підключав зараз усі можливі заклади, де є лабораторні аналізатори, це приватні лабораторії, інші лікарні та громадські організації, які займаються, наприклад ВІЛ/СНІДом і займаються тестуванням проти інших вірусів", - пояснює Павло Ковтонюк.
+Інша проблема України, за його словами, - загалом система виявлення covid-19.
+"Зараз у нас тести роблять лише, якщо ти потрапляєш до лікарні. При чому тебе туди покладуть, навіть якщо у тебе помірні симптоми. Це неправильно", - переконаний фахівець.
+На його думку, має бути система пунктів, де людям доволі масово роблять тести, навіть при легких симптомах. "Що масовіше це відбувається - то краще", - впевнений Ковтонюк.
+За його словами, тестування лише в лікарні - це постфактум фіксування тяжких випадків.
+"Добре, що приїхали тести. Але радіти рано - треба розгортати систему тестування", - резюмує Павло Ковтонюк.
+МОЗ України нагадує: якщо у вас є ознаки гострого респіраторного захворювання - телефонуйте до свого сімейного лікаря.
+Лікар ухвалює рішення, про те, робити тест чи ні, у кожному окремому випадку.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Що відбувається в "Борисполі", куди прибувають евакуйовані українці</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пасажири, які прибувають до міжнародного аеропорту "Бориспіль", проходять медичну перевірку.
+Експрес-тестування триває декілька хвилин. Мета цих заходів - запобігання поширенню коронавірусу.
+Перевіряють пасажирів, які прибули "із загрозливих напрямків".
+З 24 березня уряд припинив діяльність усіх аеропортів в Україні, окрім "Борисполя". Зараз прибуття - з одного терміналу, а відліт - з іншого.
+Пропустити Youtube допис , автор: BBC News Україна
+Увага: інші сайти можуть містити рекламу
+Кінець Youtube допису , автор: BBC News Україна
+Відео BBC News Україна в будь-який час - підписуйтеся на наш канал у YouTube.
+Всі випуски новин BBC News Україна на YouTube.
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Коронавірус: як правильно ізолюватися
+Коронавірус: що він робить з організмом
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Надзвичайний стан. Що це означає і які можуть бути обмеження</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+UNIAN
+В Україні активно обговорюють можливість введення надзвичайного стану. Що це таке і які додаткові обмеження він може запровадити?
+З минулого тижня інформпростором ширилися чутки, що у вівторок, 24 березня, парламент може зібратися на позачергове засідання для затвердження надзвичайного стану, а прем'єр-міністр Денис Шмигаль навіть заявляв про підготовку законопроєкту, який міг би дозволити президенту вводити режим НС одноосібно - без участі Верховної Ради.
+І хоча напередодні сам прем'єр запевнив, що потреби вводити надзвичайний стан в Україні наразі немає, частина оглядачів не виключає, що найближчим часом це питання знову може опинитися в порядку денному.
+РЕКЛАМА
+Пояснюємо, що таке режим надзвичайного стану, що він може змінити і які додаткові обмеження можуть бути.
+Карантин у великому місті: як кияни їдуть на роботу за перепустками
+Коронавірусна економіка у графіках
+Що в законі?
+Хоча режим НС поки офіційно не вводили, частина обмежень, які діють в Україні з минулого тижня, мають із надзвичайним станом багато спільного - йдеться, передусім, про обмеження перетину кордону і руху транспорту.
+Проте в разі офіційного запровадження режиму НС можуть з'явитися й додаткові обмеження - приміром, особливий режим в'їзду і виїзду з певних територій.
+Такі можливі заходи передбачає чинна редакція закону про надзвичайний стан:
+встановлення особливого режиму в'їзду і виїзду, а також обмеження свободи пересування по території, де вводиться надзвичайний стан
+обмеження руху транспортних засобів та їх огляд
+заборона проведення масових заходів
+заборона страйків
+примусове відчуження або вилучення майна у юридичних та фізичних осіб
+Копирайт изображения
+UNIAN
+Окрім того, в окремих ситуаціях, до яких можна віднести й поширення коронавірусу, влада може вдатися до додаткових заходів. Серед яких:
+тимчасова чи безповоротна евакуація людей з місць, небезпечних для проживання
+встановлення "квартирної повинності" для розміщення евакуйованих
+запровадження особливого порядку розподілення продуктів харчування і предметів першої необхідності
+зміна режиму роботи підприємств, переорієнтація їх на виробництво необхідної продукції
+Як запроваджують надзвичайний стан?
+За чинним законом, надзвичайний стан запроваджується указом президента, який протягом двох днів має затвердити Верховна Рада.
+При цьому в указі про надзвичайний стан президент має чітко:
+обґрунтувати його необхідність
+визначити території, на яких він вводиться
+надати перелік і межі надзвичайних заходів, вичерпний перелік конституційних прав і свобод людини й громадянина, які тимчасово обмежуються
+Закон також диктує і часові обмеження для надзвичайного стану: його можна вводити щонайбільше на місяць, і потім подовжувати ще на 30 днів - але так само за згоди Верховної Ради.
+Копирайт изображения
+UNIAN
+Надзвичайний стан і надзвичайна ситуація - в чому різниця?
+На тлі поширення епідемії коронавірусу в кількох українських областях вже запровадили режим надзвичайної ситуації, який не варто плутати із режимом надзвичайного стану.
+Режим надзвичайної ситуації запроваджується в країні або на окремих територіях в разі "порушення нормальних умов життя населення" - це може бути, приміром, епідемія, стихійні лиха, катастрофи тощо.
+В разі оголошення надзвичайної ситуації влада має змогу організовувати санітарно-епідеміологічні заходи, проводити евакуацію, посилювати охорону громадського порядку, призупиняти роботу підприємств тощо.
+Ключова відмінність від надзвичайного стану - режим надзвичайної ситуації жодним чином не обмежує конституційні права і свободи людей.
+Натомість надзвичайний стан - це особливий правовий режим, за якого ці права можуть тимчасово обмежуватися - як-от свобода пересування, свобода зібрань тощо.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Туберкульоз на волі: чому в Україні скорочують тубдиспансери</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+UNIAN
+В Україні закривають всі тубдиспансери, хворі на туберкульоз кашляють на вулицях і заражають всіх навколо - такі побоювання висловлюють у соцмережах. Чи правда це і яка зараз ситуація із цією хворобою, дізналась ВВС News Україна.
+Перш ніж почути діагноз "туберкульоз" і почати приймати ліки, Тетяна Іванова пройшла всі кола пекла.
+Вісім місяців болю в усьому тілі і температури, сотні аналізів і оглядів.
+Так довго їй не могли поставити точний діагноз.
+На рентгені легені були чисті. У неї був туберкульоз лімфовузлів.
+Що треба знати про туберкульоз
+"Чому мій терапевт не відправила мене на ретельне обстеження на туберкульоз? Вона думала, що туберкульозом хворіють лише безхатьки, наркомани і люди з в'язниць? Туберкульоз - це ж не лише кашель", - говорить пані Іванова, яка працює в благодійній організації "Конвіктус Україна".
+За даними ВООЗ, в Україні щороку своєчасно не виявляють 23% випадків туберкульозу.
+Це є причиною його подальшого поширення.
+В січні 2020 року в Україні зареєстрували 2,4 тисячі нових хворих на туберкульоз. У лютому нових випадків було 2 000. А загалом від хвороби минулого місяця лікувались 20 тисяч людей.
+В 2018 році, за даними МОЗ, в Україні було 62,3 хворих на туберкульоз на 100 000 населення.
+У цей час у Польщі, за даними Світового банку, лише 16 хворих на сто тисяч наслення, у Білорусі - 31, у Словаччині - 6.
+Більше, ніж у нас, наприклад, хворих на туберкульоз було в Афганістані, Камбоджі, Гані.
+Чому все так погано?
+"Не вистачає сучасного обладнання, яке б дозволяло швидко діагностувати туберкульоз, люди не довіряють лікарям і не звертаються вчасно. Українці люблять займатися самолікуванням - антибіотики вільно продаються в аптеках, люди їх купують, не дотримуються схем лікування, кидають. Виникає проблема з поширенням резистентних штамів збудника", - перераховує причини Оксана Зінченко, кандидатка біологічних наук, доцент кафедри мікробіології, вірусології та біотехногії ОНУ імені І.І. Мечникова.
+Майже кожен четвертий випадок в Україні - це мультирезистентний туберкульоз (МРТБ). Тобто такий, що не піддається лікуванню протитуберкульозними препаратами першої лінії.
+За кількістю хворих із такою формою країна серед "світових лідерів", розповідає колишня очільниця МОЗ Уляна Супрун.
+Одна з причин, за її словами, - застаріла система протитуберкульозної допомоги, яка залишилась ще з часів СРСР. Складовою цієї системи є тривале лікування в диспансерах.
+"Коли ця система створювалася, не було ефективних ліків проти туберкульозу, тому пацієнтів розміщували у протитуберкульозні лікарні, диспансери або санаторії на тривалий час. Тепер такі ліки є, вони доступні в Україні, за пару тижнів їх прийому людина припиняє поширювати хворобу. Тривале перебування в стаціонарі та відсутність розділення хворих з різними формами туберкульозу збільшує ризик повторного зараження", - твердить пані Супрун.
+Копирайт изображения
+UNIAN
+Що змінити?
+В Україні працює розгалужена система протитуберкульозних закладів: станом на 2018 рік було 68 тубдиспансерів, 21 туберкульозна лікарня для дорослих і дві для дітей. Всього понад 12 тисяч ліжок.
+Тривалість лікування у таких закладах - від двох до трьох місяців. На них у 2018 році виділили 1 млрд 994 тисяч грн з бюджету. Для порівняння, на лікування інсультів — 539 млн грн.
+Змінити підходи до хворих намагалися задовго до Супрун. Програму реформування протитуберкульозних закладів Верховна Рада ухвалила ще у 2012 році. Повністю систему так і не змінили.
+В 2018 році провели "оптимізацію ліжкового фонду" тубдиспансерів. Тоді скоротили майже дві тисячі ліжок - 12,4%.
+В листопаді 2019 року уряд, який тоді очолював Олексій Гончарук, ухвалив нову концепцію розвитку системи протитуберкульозної допомоги.
+У ній йшлося про реорганізацію системи тубдиспансерів, їх злиття в один-два базові заклади на рівні області, де хворі можуть лікуватися у стаціонарі. Решту - перевести на амбулаторне у поліклініки і кабінети фтизіатрів.
+Копирайт изображения
+PHC.ORG.UA
+"Ліжка не лікують"
+В Україні немає жодного диспансеру, де б дотримувалися норм інфекційного контролю, говорить представник благодійної організації "100% ЖИТТЯ", лікар-інфекціоніст Віктор Третьяков.
+Ця організація минулого року супроводжувала понад 9 тисяч хворих на туберкульоз в Україні - волонтери підтримували хворих, привозили їм ліки і їжу.
+Сам пан Третьяков об'їздив багато тубдиспансерів. Він говорить, що у більшості з них умови жахливі, ремонти робили 30-40 років тому.
+Копирайт изображения
+UNIAN
+Image caption
+Захворіти на туберкульоз можуть всі. Лише 20% серех хворих - це соціально незахищені верстви.
+Більшість хворих за два тижні лікування перестають бути заразними, їм не потрібно далі бути в стаціонарах, говорить Третьяков.
+"Якщо людина вже не виділяє паличку, то і немає потреби. А якщо людей дуже довго тримати в стаціонарі, вони заражають один одного. Наприклад, там лікується вже знебацилена людина, а поступає хтось, хто виділяє бактерії. Так з'являються резистентні форми хвороби", - пояснює лікар.
+Лікування у тубдиспансерах і туберкульозна лікарнях може тривати до 100 днів.
+"Ліжка не лікують туберкульоз, і госпіталізація хворого "в ліжко" не пов'язана з ефективністю його лікування", - підтримує реформу ТБ галузі Наталія Гранкіна, медична директорка Дніпропетровської обласної фтізіатрії.
+За її словами, туберкульоз можна лікувати амбулаторно, використовуючи міжнародні підходи, наприклад, новітні протитуберкульозні препарати, які дозволяють вилікувати резистентні форми за 9-12 місяців замість 24-36 місяців у ліжку.
+При цьому хворий не зобов'язаний весь цей час перебувати у стаціонарі. Пані Гранкіна розповідає про лікування на Дніпровщини хворих за допомогою інтерактивних дистанційних методів - хворий щодня надсилає відео своєму лікарю.
+Вона також відверто говорить, що часто стаціонарні заклади не відповідають міжнародним стандартам.
+Протитуберкульозні диспансери повинні мати споруди, які очищають і видають назовні чисту знезаражену воду.
+"Очисні споруди у нас є лише в обласному протитуберкульозному диспансері. У місті Павлоград Дніпропетровської області, наприклад, таких споруд немає. Більш того, ми мали немалу кількість проблем із павлоградським водоканалом щодо стічних вод".
+Павлоградський протитуберкульозний диспансер розташований на околиці міста. Зовні це звичайна пострадянська будівля, яких так багато у маленьких містечка: три поверхи, сіра цегла, дерев'яні вікна, давній ремонт, меблі ще з часів СРСР.
+Цей тубдиспансер обслуговвав місто Павлоград, а також весь Павлоградський та Межівський райони.
+Раніше у ньому стаціонарно лікували хворих на туберкульоз, тепер тут лише поліклініка, куди можна прийти на консультації. Якщо треба в лікарню - хворих відправляють у Кривий ріг чи Дніпро.
+"Як тепер лікуватимуться пацієнти із відкритою формою? Як можна проконтролювати лікування?", - обурюється лікарка-фтизіатр Тетяна Шишкіна, яка працювала у Павлоградському тубдиспансері.
+Вона категорично проти закриття таких закладів.
+Копирайт изображения
+ВВС
+Image caption
+Павлоградський протитуберкульозний диспансер
+За її словами, за останні три роки сюди до стаціонарних відділень госпіталізували 919 хворих із відкритою формою, з них 543 - це люди, що мали стійку форму туберкульозу, яку лікують довго і яку потрібно контролювати.
+"Одна людина із відкритою формою, якщо вона не проходить лікування, може заражати до 15 людей. Тобто уявіть потенційне число заражених! Якщо заклад закриватимуть, то ми можемо говорити про можливий початок епідемії в місті", - обурюється пані Шишкіна.
+Хворих не виганятимуть на вулицю, стаціонар працює далі, але ліжка будуть максимально сконцентровані на базі обласного Дніпропетровського протитуберкульозного диспансеру і диспансеру Кривого Рогу, відповідає пані Гранкіна.
+Згідно з реформою, у кожній області має залишитись мінімум один великий заклад — фтизіатричний центр або центр легеневих хвороб, де можна лікуватися на стаціонарі.
+Головне, щоб ці заклади розміщувалися не на далекій відстані й хворі могли до них доїхати, говорить пан Третьяков з "100% ЖИТТЯ".
+Також продовжать роботу кабінети фтізіатрів у районах, де пацієнти зможуть отримувати ліки. Крім того, у планах уряду - ввести посади міжрайонних фтизіатрів у регіональних центрах.
+Директорка Дніпропетровської фтізіатрії говорить, що амбулаторна служба працюватиме в області й надалі, і саме ці фтизіатри будуть відповідати за виявленням хворих.
+Але реформа лікування туберкульозу, як і вся медреформа, може опинитися під питанням через зміну керівництва МОЗ і ситуацію з коронавірусом.
+Лікар-інфекціоніст Віктор Третьяков пояснює: коронавірус може погіршити ситуацію з туберкульозом тому, що потенційно хворі на ТБ - якраз у групі ризику.
+"Це може збільшити смертність", - говорить лікар.
+Копирайт изображения
+UNIAN
+Стигма
+Боротьба Тетяни Іванової з хворобою тривала два роки і три місяці.
+Зараз вона видужала і тепер розповідає про свій досвід, виступає на тренінгах і семінарах, присвячених туберкульозу, закликає долати стигму довкола цієї хвороби.
+"Один з важливих пунктів лікування від туберкульозу - не боятися говорити. Я думала, що ця хвороба - це все, це вирок. Але це ж не так", - каже Тетяна Іванова під час свого виступу на тренінгу організації "Зупинимо туберкульоз. Україна".
+В Україні, яка серед лідерів у Європі з поширення туберкульозу, навколо цієї хвороби справді багато міфів, неперевіреної інформації та страхів.
+"Чому ж, коли є ефективні ліки, в Україні так багато хворих? Для багатьох людей страшно визнати, що у тебе туберкульоз. Страшно піти лікуватись. Страшно відчувати себе відчуженим, - говорить лікарка Гунта Дравніце, голова проєкт "Підтримка зусиль у протидії туберкульозу в Україні", - Туберкульоз - виліковний. Це варто пам'ятати".
+За участю позаштатного кореспондента ВВС News Україна Артема Лисенка
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ШВЛ: що це і чи справді бракує систем</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+На тлі пандемії коронавірусу у світі дедалі частіше говорять про жорстку нестачу систем штучної вентиляції легень (ШВЛ). Пояснюємо, що це таке і навіщо вони потрібні.
+Що таке системи ШВЛ?
+Лише за офіційними даними, вже понад 350 тисяч людей у світі підхопили коронавірус (станом на 23 березня). І хоча переважна більшість інфікованих переносять хворобу в легкій формі та зрештою одужують, в частині випадків у пацієнтів виникають серйозні ускладнення.
+Одне із таких ускладнень - стан, коли людина не може дихати самостійно. Точніше, її дихання настільки слабке, що не забезпечує достатнього надходження кисню до організму.
+Саме щоб підтримувати життя хворого в таких умовах, потрібні апарати штучної вентиляції легень.
+"Коли тобі кажуть: у тебе - коронавірус". Розповідь першого українця, який одужав
+Коронавірус: що він робить з організмом
+У коронавіруса є суперпоширювачі. Хто вони такі?
+Таке обладнання може використовуватися як під час операцій, коли пацієнт упродовж кількох годин перебуває під наркозом, так і для довгострокової підтримки дихання.
+Іноді системи штучної вентиляції не допомагають: концентрація кисню в крові хворого лишається невисокою і його доводиться переводити на так звану екстракорпоральну мембранну оксигенацію (ЕКМО). Під час цієї процедури кров пацієнта пропускають через спеціальний пристрій, який насичує її киснем і повертає назад.
+Проте обладнання для ЕКМО застосовується лише у виняткових випадках, коштує дорожче, а сама процедура потребує спеціально навчених фахівців, тоді як системи ШВЛ вважаються більш універсальним методом.
+У чому проблема?
+В тому, що апаратів ШВЛ в Україні небагато. До того ж, частина цього обладнання технологічно застаріла і потребує оновлення: з-поміж іншого, апарати нових зразків мінімізують кількість випадків пошкодження легень, спричинених механічною вентиляцією.
+За словами головного державного санітарного лікаря Віктора Ляшка, в українських відділеннях інтенсивної терапії наразі налічується близько 3 500 систем ШВЛ, і якщо коронавірус і далі поширюватиметься, в якийсь момент, визнає він, такої кількості апаратів може просто не вистачити.
+Копирайт изображения
+SPL
+Image caption
+Легені, інфіковані коронавірусом
+Судячи з прогнозів учених, жодних сумнівів у тому, що вірус поширюватиметься все активніше, немає.
+Втім, як довго все це триватиме, скільки людей підхоплять коронавірус і скільки випадків будуть летальними - відповіді на ці питання носять суто теоретичний характер, адже досі незрозуміло, якою є реальна кількість інфікованих, наскільки ефективними виявляться карантинні заходи та як швидко вдасться винайти вакцину.
+Ось лише один із прогнозів від дослідників з Австралійського національного університету, які нещодавно змоделювали 7 різних сценаріїв розвитку ситуації: за найсприятливішим із них від коронавірусу помруть 15 мільйонів людей в усьому світі, за найгіршим - понад 68 мільйонів.
+Коронавірус: коли закінчиться епідемія
+Що робить Україна?
+Українська влада регулярно говорить про нові кроки у боротьбі з коронавірусом, зокрема закупівлю систем ШВЛ.
+Прем'єр-міністр Денис Шмигаль днями заявив, що в регіони направили 1,5 тисячі апаратів, Володимир Зеленський - про доставку систем штучної вентиляції із Китаю. Додаткові кошти виділяють і з місцевих бюджетів.
+Окрім того, у Києві налагодити виробництво апаратів штучної вентиляції має завод "Буревісник", який входить до концерну "Укроборонпром".
+Долучається до боротьби з коронавірусом і приватний бізнес: кошти на закупівлю кількох сотень апаратів ШВЛ виділили, зокрема, Фонд Ріната Ахметова та мережа магазинів "Епіцентр", а одеська компанія Revel Laboratory, що займається 3D-друком, пообіцяла перевести своє обладнання на виготовлення клапанів для систем ШВЛ.
+Копирайт изображения
+GETTY IMAGES
+Image caption
+Коронавірус у світі, лише за офіційними даними, підхопили понад 300 тисяч людей (станом на 23 березня)
+Не лише українська проблема
+Про дефіцит систем штучної вентиляції на тлі поширення коронавірусу говорять не лише в Україні: про проблему пишуть десятки західних ЗМІ - від CNN до The News York Times, на неї жаліються лікарі в Італії, про потенційну нестачу апаратів попереджають і в парламентському комітеті з питань охорони здоров'я Великої Британії.
+Найбільші світові виробники систем ШВЛ - компанії Medtronic Plc, Philips NV, Draegerwerk AG і Getinge AB - вже заявили, що нарощують виробництво, щоб задовольнити збільшений попит.
+Не виключили запуск виробництва ШВЛ-обладнання й автомобільні компанії General Motors і Ford Motor Company. Засновник Tesla Ілон Маск також повідомив, що його компанія займеться виробництвом апаратів штучної вентиляції легень, якщо їх бракуватиме - чого не виключають чимало експертів.
+На пропозицію Маска вже встиг відгукнутися мер Нью-Йорка Білл де Блазіо.
+"Країні вкрай не вистачає цього обладнання, і воно потрібно нам якнайшвидше - протягом кількох тижнів нам знадобляться тисячі таких апаратів, і ми не відмовилися б від вашої допомоги", - заявив де Блазіо.
+Втім, фахівці наголошують: попри усі проблеми, апарати штучної вентиляції - не універсальний спосіб перемоги над коронавірусом, і основні зусилля країн мають бути кинуті насамперед на боротьбу з поширенням хвороби.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Хроніки коронавірусу: ковзанка-морг в Іспанії та 24 нових випадків в Україні</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+Станом на ранок 24 березня кількість заражених коронавірусом у світі перевищила 381 тис. людей. Понад 16 тис. із них померли, понад 101 тис. - одужали.
+Лідерами за смертністю у світі й надалі залишаються Італія, де від коронавірусу померли понад 5 тис. людей, Китай — понад 3 тисячі та Іспанія — понад 2 тисячі.
+Скільки Україні треба тестів на коронавірус
+В Україні станом на 13:00 24 березня загалом зафіксували 97 випадків зараження коронавірусом. За минулу добу - 11 нових випадків, а за вівторок - 13 нових випадків, всі в Чернівецькій області.
+Сходив на похорон: новий випадок на Тернопільщині
+У Тернопільській області діагностували другий на регіон випадок зараження коронавірусом.
+Вірус підхопив чоловік, який був на одному похороні зі священиком, у якого також раніше діагностували цю хворобу, повідомляє Тернопільський обласний лабораторний центр.
+Закриті Штати Америки і рейси-привиди: скільки втрачає туризм через коронавірус
+Коронавірус: коли закінчиться епідемія
+Чи допомагає алкоголь? Топ-5 міфів про коронавірус
+Людям, які контактували з хворим, рекомендували самоізолюватись.
+Права на зображення BBC News Україна
+BBC NEWS УКРАЇНА
+Італія: позитивні зрушення
+В Італії, яка найбільше серед усіх європейських країн постраждала від коронавірусу, схоже, почали спостерігати позитивну динаміку.
+Другий день поспіль кількість загиблих зменшується відносно до попереднього дня. Станом на вечір 23 березня тут загинула 601 людина проти 651 23 березня.
+Крім того, пішло на спад розповсюдження хвороби. 23 березня тут зареєстрували 4789 нових заражень коронавірусом, у два попередні дні кількість діагностованих хворих склала - 6557 та 5560 людей.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Суворий карантин в Британії
+У Великій Британії, яка довгий час зволікала з запровадженням серйозних обмежень через коронавірус, проголосили суворий карантин на найближчі три тижні.
+За словами прем'єр-міністра Британії Бориса Джонсона, британцям треба залишатися вдома.
+Виходити можна тільки в окремих випадках: щоб сходити за продуктами, отримати медичну допомогу, зайнятись спортом (не більше одного разу на день) і поїхати на роботу, якщо її неможливо зробити з дому.
+Магазини, за винятком тих, де продаються продукти і товари першої необхідності, закриють. Заборонені будь-які зібрання, де є понад дві людини.
+Покинуті і мертві пенсіонери в Іспанії
+Копирайт изображения
+GETTY IMAGES
+Image caption
+Palacio de hielo - ковзанка в Мадриді, яку владі довелось тимчасово використовувати як морг через велику кількість загиблих від коронавірусу
+В Іспанії, одній з країн-лідерів за кількістю хворих на коронавірус, військові виявили, що людей похилого віку у притулках кидає персонал. Їх знаходили покинутими та занедбаними у своїх ліжках. У деяких випадках - мертвими.
+Правоохоронні органи Іспанії розпочали розслідування.
+У понеділок в Іспанії зафіксували найвищий рівень смертності від коронавірусу - 462 людини. Загалом тут загинули понад 2 тис. людей.
+У Мадриді як морг тимчасово стали використовувати головну міську ковзанку площею 1800 кв. м.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">У депутата "Слуги народу" виявили коронавірус</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+FACEBOOK
+Руслан Горбенко, народний депутат від партії "Слуга народу", підхопив коронавірус.
+Про це ввечері у понеділок повідомила його колежанка, заступниця голови фракції Євгенія Кравчук.
+За її словами, Горбенко наразі перебуває в лікарні, в нього запалення легень.
+Коронавірус: що він робить з організмом
+У Раді підозра на другого хворого на коронавірус
+"Коли тобі кажуть: у тебе - коронавірус". Розповідь першого українця, який одужав
+"Руслан в останній місяць не виїжджав закордон, не відпочивав у куршевелях. Тобто міг заразитися лише в Україні", - написала пані Кравчук.
+Вона припустила, що своїх колег Горбенко заразити не міг, але не виключила, що деяким депутатам доведеться піти на самоізоляцію.
+Пропустити Facebook допис , автор: Yevheniya
+Кінець Facebook допису , автор: Yevheniya
+Не перший депутат
+Раніше захворювання на коронавірус офіційно підтвердилося в депутата з групи "Довіра" Сергія Шахова, який нещодавно повернувся з Європи.
+Він розповідав, що хвороба почалася з підвищення температури, після чого він одразу викликав лікарів та здав аналізи.
+Шахов також запевняв, що почувається добре.
+З підозрою на коронавірус у лікарні опинився депутат з групи "Довіра" Сергій Вельможний.
+Поки що тест у нього негативний, хоча є всі симптоми хвороби. Але тест його сина, якого госпіталізували разом з депутатом, виявився позитивним.
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">У Києві кілька годин стояв потяг із Риги. Коронавірус не виявили</t>
+  </si>
+  <si>
+    <t xml:space="preserve">На Центральному залізничному вокзалі у Києві упродовж кількох годин стояв потяг із Риги (Латвія). На ньому перебували понад 600 пасажирів.
+Потяг "Рига-Київ", про який йде мова, прибув до України в рамках евакуаціі, яку організовує МЗС Украіни, щоб повернути додому украінців, які застрягли за кордоном.
+Прессекретар Держприкордонслужби Андрій Демченко в коментарі BBC News України розповів, що на потязі також були кілька іноземців - вони мають посвідку на проживання в Україні.
+Карантин у великому місті: як кияни їдуть на роботу за перепустками
+Кожному пасажиру вимірювали температуру і запитували про самопочуття, в разі підозри на коронавірус - проводили експрес-тест.
+Як повідомляють у МОЗ, підозру встановили 5 людям, але зрештою не підтвердився жоден випадок захворювання Covid-19.
+Близько 20:45 стало відомо, що пасажирів випустили з потяга.Усі пасажири, за словами Андрія Демченка, підписали добровільну згоду на самоізоляцію.
+Права на зображення BBC News Україна
+BBC NEWS УКРАЇНА
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Олександр Пономарів</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Блог Пономарева: коронавірус чи короновірус?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+UNSPLASH
+Доктор філологічних наук Олександр Пономарів відповідає на запитання читачів.
+Запитання від редакції. Як правильно: коронавірус чи короновірус? Інтуїтивно хочеться написати короновірус, бо в українській складні іменники часто творяться за допомогою сполучного звука о, як-от газогін, верболіз.
+Слово coronavirus створено 1968 року від латинських слів corona ("вінець") та virus ("отрута"). Його механічно перенесено в українську мову з написанням без дефіса, отож - коронавірус.
+Петро Жижиян цікавиться, як писати слово мережа, коли йдеться про Інтернет, - з великої чи малої літери.
+З великої.
+Дар'я Задорожна хоче знати, звідки походить ім'я Миколай (ідеться про святого) в українській мові, коли активно побутує ім'я Микола, і той кінцевий -й не має грецького походження.
+Ім'я Миколай походить від грецького Νικόλαος. В українській мові воно вживане як найменування святого.
+Кінцевий -й з'явився на місці грецького закінчення -оς (пор. грецьке Αλέχιος - Олексій, або латинське Sergius - Сергій).
+У нерелігійному вживанні в українців поширена форма Микола.
+Звертання від читача Тимофія. Чи можна замінити чимось більш українським популярне нині слово крафтовий, як-от у словосполученні крафтова продукція?
+Поки що питомого українського відповідника немає. Частина крафт (від німецького Kraft - сила) є одним зі складників у словах: крафтакробат, крафтцелюлоза, крафтпапір тощо.
+Відомий англійський вислів фейспалм, що означає жест розчарування, навіть роздратування, чомусь передають як рукалице в українському просторі. Чи можна знайти відповідник у нашій мові, що пасує краще?
+Поки що такого відповідника немає.
+Чи є різниця між крапати та капати? Словники подають обидва слова, хоч мене, пише читач, навчали, що саме крапати й крапля є більш питомими в українській мові. Нещодавно натрапив на слово викапаний, яке рекомендують використовувати замість російського вылитый, але я ніколи не чув слова викрапаний.
+Крапля і капля - морфологічні синоніми. Проте більш український - крапля, тому його використовують частіше й у вільному, і в фразеологічному вжитку. Краплі - в медицині, крапельниця; у висловах до останньої краплі, як дві краплі води, як крапля в морі й под.
+Але коли хтось на когось дуже схожий, - традиційно кажемо викапаний: дочка - викапана мати.
+Чи правильно вживати слово в'яжучий, як от в'яжучий засіб?
+Правильно - в'язкий засіб.
+----
+Будь ласка, зверніть увагу, що професор Пономарів користується Проєктом українського правопису 1999 року, тож слова на кшталт инший чи варіянт - це не помилки.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Хроніки коронавірусу: у світі 350 тисяч хворих, Balenciaga та Yves Saint Laurent шитимуть маски</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+23 березня кількість заражених коронавірусом в світі перевищила 350 тисяч людей. Понад 15 тисяч із них померли, понад 100 тисяч - одужали.
+Лідерами за смертністю у світі й надалі залишаються Італія (понад 5 тисяч смертей), Китай (понад 3 тисячі) та Іспанія (понад 2 тисячі).
+Закриті Штати Америки і рейси-привиди: скільки втрачає туризм через коронавірус
+Знаменитості, які підхопили коронавірус
+Balenciaga та Yves Saint Laurent шитимуть маски
+Французька корпорація Kering повідомила, що майсетрні фешн-брендів Balenciaga та Yves Saint Laurent, які їй належать, займуться виробництвом медичних масок.
+Окрім того, в компанії розповіли, що найближчими днями передадуть французькій владі три мільйони масок, закуплених в Китаї.
+Також Kering повідомила про пожертву на користь Інституту Пастера в Парижі - для підтримки досліджень коронавірусу COVID-19.
+Заразилися: Гарві Вайнштейн та Пласідо Домінго
+Копирайт изображения
+GETTY IMAGES
+Скандальний голлівудський продюсер Гарві Вайнштейн заразився коронавірусом. Це підтвердило тестування.
+В лютому його визнали винним у зґвалтуванні та сексуальних насильствах і засудили до 23 років ув'язнення.
+Вайнштейн наразі перебуває у виправному закладі Венде, його відправили в ізоляцію, щоб він не заразив інших в'язнів.
+Також в неділю підтвердив, що захворів на коронавірус, 79-річний іспанський оперний співак Пласідо Домінго.
+Співак запевнив, що почувається добре, але перебуває у самоізоляції разом з родиною.
+Ангела Меркель - на карантині
+Канцлерка Німеччини Ангела Меркель у неділю оголосила, що йде на карантин, оскільки у п'ятницю вона зустрілася з лікарем, в якого пізніше діагностували коронавірус.
+Також з метою боротьби з розповсюдженням пандемії уряд Німеччини заборонив зустрічі більш як двох людей поза роботою та домом протягом двох тижнів.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Бунти в колумбійських в'язницях
+Щонайменше 23 в'язні загинули під час бунту у в'язниці Боготи. 83 отримали поранення.
+Заворушення спричинила напруга через поширення коронавірусу. В'язні по всій країні протестують проти перенаселеності закладів позбавлення волі та поганої медичної допомоги.
+Канада відкликає атлетів, Олімпіада під загрозою
+Канада слідом за Австралією офіційно визнала, що через коронавірус не відправить своїх атлетів на Олімпійські ігри в Токіо, проведення яких запланували на липень-серпень цього року.
+Спортсменам рекомендували готуватися до участі в Олімпіаді у 2021 році.
+Таке рішення Канади ще більше ставить під сумнів, що ігри цього року взагалі відбудуться.
+Міжнародний олімпійський комітет пообіцяв ухвалити рішення щодо Олімпіади 2020 - в найближчі чотири тижні.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ходити в храм чи ні: що каже церква про карантин</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+УНІАН
+Image caption
+Митрополит УПЦ МП Павло закликав людей ходити до храму
+Релігійні діячі загалом закликають своїх вірян дотримуватися вимог карантину через коронавірус.
+В розпал пандемії найвпливовіші церкви України озвучили свої рекомендації, серед яких не піддаватися паніці, дотримуватися правил гігієни, а за необхідності залишатися вдома і дивитися трансляцію богослужінь.
+Утім є й такі церковники, які закликають під час карантину "не боятися і ходити в церкву". Наскільки це безпечно та чи порушують такі священики правила карантину?
+З'їздили в Почаїв: молдовські паломники "імпортували" коронавірус з України
+Не цілувати і не цілуватись: як не заразитись коронавірусом у церкві
+"Моліться, постіться, ходіть у храм"
+13 березня на YouTube каналі Києво-Печерської Лаври з'явилося відеозвернення митрополита УПЦ МП Павла під назвою "Карантин: чи скасують богослужіння".
+У ньому настоятель Лаври заявив, що "найстрашніша епідемія - це гріх, який руйнує людську природу".
+"Не бійтесь нічого, не жахайтеся подій, які йдуть - а вони будуть, і буде ще гірше, якщо ми не покаємося", - наголосив владика Павло.
+"Від нас сьогодні потрібне єдине: моліться, постіться, ходіть у храм, причащайтесь і причащайте дітей маленьких. Не дивіться: старше покоління чи молодше. Всі поспішайте до храму", - закликав священник.
+Він також розкритикував "укази безумних велінь, щоб сьогодні не ходили до храмів".
+Права на зображення ЛАВРА. ПУТЬ СПАСЕНИЯ
+ЛАВРА. ПУТЬ СПАСЕНИЯ
+"Ми живемо у вільній, як називають сьогодні, демократичній країні. І ніхто не має права змусити мене не ходити до храму", - відзначив митрополит Павло.
+Він також запевнив, що не дозволить закрити Києво-Печерську Лавру: "Ми будемо ходити хресними ходами, будемо цілодобово молитися".
+Як проходять богослужіння
+За кілька днів, вже після введення жорстких заходів карантину про обмеження зібрань, митрополит Павло записав друге відеозвернення, де вже трохи пом'якшив позицію щодо церковних ритуалів під час карантину.
+"Якщо людина боїться цілувати ікону, то можна просто нахилити голову", - пояснив він.
+Митрополит також відзначив, що можна не цілувати руку священнику.
+Права на зображення ЛАВРА. ПУТЬ СПАСЕНИЯ
+ЛАВРА. ПУТЬ СПАСЕНИЯ
+При цьому Священний синод УПЦ МП закликав своїх вірян все ж не ходити до церкви, якщо з'явилися симптоми хвороби, не збирати на богослужіння більше десяти людей, а в ритуалах використовувати одноразовий посуд.
+"Потрібно ретельно стежити, щоб ікони, до яких прикладаються вірні, постійно протиралися дезінфекуючим розчином", - йдеться у рішенні синоду.
+Дотримуватися карантину закликали й в інших конфесіях. Утім повністю від богослужінь не відмовилися - наприклад, у православних зараз період перед Великоднем, на який припадає багато літургій.
+Предстоятель ПЦУ митрополит Епіфаній у неділю провів службу у Свято-Михайлівському соборі Києва. На фото видно, що на ній було більше десяти людей.
+Копирайт изображения
+POMISNA.INFO
+А перший випадок коронавірусу на Тернопільщині стався у священника греко-католицької церкви, який до госпіталізації встиг провести кілька богослужінь і похорон, та навіть сходити в райдержадміністрацію.
+Про свою хворобу він, вочевидь, не знав. Інакше за це могла б бути кримінальна відповідальність.
+Що кажуть у поліції
+Джерела BBC News Україна у Національній поліції кажуть, що не вважають заклики священників ходити в церкву порушенням норм щодо карантину.
+Там додають, що відповідальність могла б бути, якби якісь релігійні діячі свідомо закликали порушувати карантинні обмеження і не довіряти уряду.
+Або ж хтось зі священників проводив богослужіння, знаючи про свою хворобу.
+Копирайт изображения
+НАЦІОНАЛЬНА ПОЛІЦІЯ
+Водночас у поліції кажуть, що готові розглянути заяву про порушення релігійних діячів, наприклад, про проведення богослужіння за участі понад десяти людей, якщо таку заяву хтось подасть.
+Поліція вже склала півтори тисячі адмінпротоколів за статтею про "порушення правил щодо карантину людей".
+"У разі виявлення порушень умов карантину просимо громадян повідомляти на спецлінію 102 для негайного реагування", - закликають правоохоронці.
+Секта у Кореї
+Копирайт изображения
+EPA
+Image caption
+Лідер секти, через яку поширився коронавірус у Південній Кореї, вибачався на колінах
+Тим часом у Південній Кореї збираються судити лідерів секти "Храм скинії свідоцтва Шинь-Чонджу", яких звинувачують у поширенні коронавірусу.
+За даними офіційних осіб, спалах коронавірусу у Кореї почався з міста Тегу, де послідовники цієї секти заразили один одного під час обряду, після чого вірус почав поширюватися по країні.
+Лідер секти - 88-річний Лі Ман Хі - називає себе біблійним месією. Він стверджує, що "судний день" настане за його життя, і тоді 144 тисячі його послідовників піднімуться разом з ним на небеса.
+Він вже вибачився на колінах перед нацією: "Хоча це не було зроблено навмисно, багато заразилися. Ми намагалися, як могли, щоб запобігти цьому, але у нас не вийшло".
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+УНІАН
+У першому уряді за президента Зеленського керівника МВС Арсена Авакова називали "тимчасовим міністром", який пропрацює кілька місяців.
+Утім, тимчасовим виявився Кабмін Гончарука, тоді як Аваков залишився працювати в новому уряді Шмигаля і відзначив шість років на посаді міністра внутрішніх справ.
+Надзвичайний стан. Що це означає і які можуть бути обмеження
+Як коронавірус шириться планетою. Мапа
+Зараз його вже не називають "тимчасовим", він керує найпотужнішою структурою в умовах карантину і радить Верховній Раді та всьому уряду, що треба зробити в економіці.
+А також - готує суспільство до введення надзвичайного стану, який ще більше розширить повноваження його міністерства.
+Силовики і карантин
+Копирайт изображения
+МВС
+Арсена Авакова називали однією з проблем формування уряду Дениса Шмигаля. Через це, зокрема, за новий Кабмін голосували пакетом, адже не факт, що при поіменному голосуванні за кожного з міністрів знайшлося б достатньо голосів.
+Утім, з початком спалаху коронавірусу в Україні керівник МВС став однією з ключових фігур не тільки в Кабміні, але й у державі загалом.
+Поліція та інші підрозділи, які входять до структури міністерства внутрішніх справ - Нацгвардія, Держслужба з надзвичайних ситуацій і Прикордонна служба - зараз мають головну роль у всіх карантинних заходах.
+Копирайт изображения
+МВС
+Відділення спецобробки ДСНС проводить знезараження у Радомишлі, де був один з перших підтверджених випадків коронавірусу в країні, авіація Нацгвардії доправляє з Китаю тести та костюми хімзахисту, а поліцейсьі у великих містах стежать, кого і скільки перевозить громадський транспорт.
+З подачі МВС посилена відповідальність за порушення карантину — за це тепер штрафи від 17 до 32 тис. грн.
+Крім того, за навмисне зараження коронавірусом інших людей можна потрапити до в'язниці на строк до восьми років. У МВС пояснюють, що в'язниця загрожуватиме лише тим, хто точно знав про свою хворобу і свідомо заражав нею інших, наприклад, у транспорті.
+На пів дорозі до надзвичайного стану?
+Копирайт изображения
+МВС
+МВС стало локомотивом введення надзвичайної ситуації в областях, де виявили коронавірус.
+За Кодексом цивільного захисту населення - це етап, який може передувати надзвичайному стану.
+Арсен Аваков нещодавно написав, що у найближчі дні обмеження "будуть значно жорсткішими".
+За його словами, це потрібно, щоб виграти час для системи охорони здоров'я: "Кожен день не надмірної напруги нашої перехідної, кульгавої медичної системи — важливий!"
+Пропустити Facebook допис , автор: Arsen
+Дорогие украинцы! События последних дней кардинально изменили жизнь всего общества и всего мира. Мир меняется и...
+Posted by Arsen Avakov on Saturday, 21 March 2020
+Кінець Facebook допису , автор: Arsen
+Про те, що вже введені обмеження недостатні, говорять й інші люди з команди Авакова.
+"Все буде залежати від статистики, зокрема смертності... Попереду у нас буде піт, кров і сльози, як казав прем'єр-міністр Британії Вінстон Черчилль перед Другою світовою війною", - заявив у "Свободі слова" на ICTV заступник міністра внутрішніх справ Антон Геращенко.
+Він також порівняв нинішній спалах коронавірусу з епідемією "іспанки" у 1918-1919 роках, від якої загинули кілька десятків мільйонів людей.
+Антон Герщенко попередив тих, хто вже міг заразитися (наприклад, повернувся з-за кордону), що вони мають дотримуватися самоізоляції.
+"Поліція почала централізовано отримувати контакти з ваших анкет. За необхідності будемо звертатися до мобільних операторів, будемо звертатися до банківської сфери. Ви зобов'язані перебувати вдома, щоб зберегти життя своїх близьких", - закликав заступник міністра.
+І додав: "У нас карантин зараз на 50-60%. В Італії та Іспанії — на 95%... Ми до цього часу зупинилися на пів дорозі. І продовжується величезне спілкування людей з людьми".
+За даними BBC News Україна, Верховна Рада може винести на голосування надзвичайний стан вже цього тижня.
+Він - значно суворіший за нинішні надзвичайні ситуації і може передбачати серйозні обмеження, аж до блокпостів і заборони руху на особистому транспорті між містами. Видання Insider також писало про плани запровадити можливість комендантської години та обшуків під час пандемії.
+Контролюватимуть дотримання надзвичайного стану, якщо його коли-небудь все ж запровадять, саме структури МВС.
+Водночас у вівторок ввечері Арсен Аваков у коментарі "Українській правді" запевнив, що наразі не бачить сенсу у запровадженні надзвичайного стану.
+"Для забезпечення карантину нам цілком досить оголошення режиму надзвичайної ситуації, який зараз діє в Києві і інших містах… Надзвичайний стан зараз не потрібен. Він передбачає обмеження конституційних прав. Для боротьби з вірусом нам це ні до чого. Його запровадження може бути тільки крайнім заходом", - пояснив міністр.
+А що з економікою?
+Паралельно Арсен Аваков почав давати поради уряду та парламенту у сферах, які виходять за межі його компетенції як міністра внутрішніх справ - в економіці та фінансах.
+Він закликав переглянути Держбюджет, значно збільшити його дефіцит, укласти угоду з МВФ та реструктуризувати зовнішні борги, щоб менше виплачувати у найближчі роки.
+"Без цих та інших екстраординарних заходів буде жахливо складно! Людям буде дуже складно! І тому треба діяти, захищаючи людей, балансуючи економіку в умовах, яких ще не було", - наголосив Аваков.
+"Вимушена необхідність"
+Копирайт изображения
+УНІАН
+"Посилення ролі Арсена Авакова у часи кризи, пов'язаної з пандемією, я називаю "вимушеною необхідністю". В умовах, коли урядовці не знають, що робити з кризою, активність Авакова я вважаю позитивом", - говорить BBC News Україна політичний консультант Петро Охотін.
+Петро Охотін додає, що МВС ще з часів Леоніда Кучми має чи не найбільш чітку і дієву вертикаль серед усіх інших державних інститутів.
+"Роль Арсена Авакова зростає в умовах, коли інші чиновники намагаються взяти на себе якомога менше відповідальності, адже Кабмін Дениса Шмигаля формувався не як антикризовий, а радше як консенсусний", - відзначає політичний консультант.
+"З одного боку, фігура Авакова не раз піддавалася критиці. З іншого, просто уявіть, що Арсен Борисович зараз вирішить піти у відставку. Очевидно, що слабкість державної вертикалі і некомпетентність команди Зеленського створює всі умови для приходу сил, готових до більш авторитарних дій. Ще давні греки казали: "анархія - мати порядку", адже після хаосу часто встановлювалися тиранії", - вважає Петро Охотін.
+Новий фаворит
+Копирайт изображения
+УНІАН
+Керівник аналітичної групи "Левіафан" Микола Мельник каже, що політична вага Арсена Авакова поступово зростала протягом президентства Зеленського.
+"Роль Авакова аномально зросла не сьогодні, це був доволі тривалий процес, що розпочався з моменту формування коаліційного уряду Гончарука. А потім комом зростав до пресконференції щодо "призначення" винних у справі Шеремета", - пригадує аналітик.
+У МВС наполягають, що не "призначали" нікого винним у цій справі, а лише говорили про людей, які "обгрунтовано підозрюються" у причетності до вбивства журналіста. Тим не менше, згадана пресконференція, ще й за участі глави держави, викликала значний резонанс та критику через наведені докази, які захист затриманих вважає сумнівними.
+Поліція затримала підозрюваних у справі Шеремета. Серед них музикант Riffmaster?
+"Потім роль Авакова у державницьких процесах лише зростала, адже слід пам'ятати, що Аваков - це не тільки МВС, це і Мінінфраструктури та пару десятків депутатів у парламенті", - додає Микола Мельник.
+На його думку, роль Арсена Авакова буде зростати, поки Володимир Зеленський "буде вбачати в українцях, які його не підтримують, загрозу".
+"А картинка для цього створюється ідеальна. Це і "падіння Сивохи", і "бійки за землю" на Грушевського, і заяви волонтерки" Звіробій та депутатки Федини", - додає аналітик.
+На його думку, найбільше сила Авакова зросте якраз із введенням надзвичайного стану: "Адже саме на нього буде покладене його дотримання".
+"Він суто психологічно сильніший за всіх в оточенні президента і вміє переконувати Зеленського в своїй правоті. Чим, до речі, можуть похвалитись одиниці", - відзначає Мельник.
+За його словами, Аваков вже вписався у схему "фаворитів" Зеленського, яку раніше очолював Андрій Богдан і яка існує через "вакуум влади" навколо президента.
+"Можливо, цей вакуум виникає через те, що Зеленський щиро намагається побудувати систему управління шляхом корпоративного делегування повноважень. А в умовах української традиції держуправління це сприймається як слабкість. Кожен намагається цей вакуум заповнити", - резюмує Микола Мельник.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+UNIAN
+В Україні активно обговорюють можливість введення надзвичайного стану. Що це таке і які додаткові обмеження він може запровадити?
+З минулого тижня інформпростором ширилися чутки, що у вівторок, 24 березня, парламент може зібратися на позачергове засідання для затвердження надзвичайного стану, а прем'єр-міністр Денис Шмигаль навіть заявляв про підготовку законопроєкту, який міг би дозволити президенту вводити режим НС одноосібно - без участі Верховної Ради.
+І хоча напередодні сам прем'єр запевнив, що потреби вводити надзвичайний стан в Україні наразі немає, частина оглядачів не виключає, що найближчим часом це питання знову може опинитися в порядку денному.
+Пояснюємо, що таке режим надзвичайного стану, що він може змінити і які додаткові обмеження можуть бути.
+Карантин у великому місті: як кияни їдуть на роботу за перепустками
+Коронавірусна економіка у графіках
+Що в законі?
+Хоча режим НС поки офіційно не вводили, частина обмежень, які діють в Україні з минулого тижня, мають із надзвичайним станом багато спільного - йдеться, передусім, про обмеження перетину кордону і руху транспорту.
+Проте в разі офіційного запровадження режиму НС можуть з'явитися й додаткові обмеження - приміром, особливий режим в'їзду і виїзду з певних територій.
+Такі можливі заходи передбачає чинна редакція закону про надзвичайний стан:
+встановлення особливого режиму в'їзду і виїзду, а також обмеження свободи пересування по території, де вводиться надзвичайний стан
+обмеження руху транспортних засобів та їх огляд
+заборона проведення масових заходів
+заборона страйків
+примусове відчуження або вилучення майна у юридичних та фізичних осіб
+Копирайт изображения
+UNIAN
+Окрім того, в окремих ситуаціях, до яких можна віднести й поширення коронавірусу, влада може вдатися до додаткових заходів. Серед яких:
+тимчасова чи безповоротна евакуація людей з місць, небезпечних для проживання
+встановлення "квартирної повинності" для розміщення евакуйованих
+запровадження особливого порядку розподілення продуктів харчування і предметів першої необхідності
+зміна режиму роботи підприємств, переорієнтація їх на виробництво необхідної продукції
+Як запроваджують надзвичайний стан?
+За чинним законом, надзвичайний стан запроваджується указом президента, який протягом двох днів має затвердити Верховна Рада.
+При цьому в указі про надзвичайний стан президент має чітко:
+обґрунтувати його необхідність
+визначити території, на яких він вводиться
+надати перелік і межі надзвичайних заходів, вичерпний перелік конституційних прав і свобод людини й громадянина, які тимчасово обмежуються
+Закон також диктує і часові обмеження для надзвичайного стану: його можна вводити щонайбільше на місяць, і потім подовжувати ще на 30 днів - але так само за згоди Верховної Ради.
+Копирайт изображения
+UNIAN
+Надзвичайний стан і надзвичайна ситуація - в чому різниця?
+На тлі поширення епідемії коронавірусу в кількох українських областях вже запровадили режим надзвичайної ситуації, який не варто плутати із режимом надзвичайного стану.
+Режим надзвичайної ситуації запроваджується в країні або на окремих територіях в разі "порушення нормальних умов життя населення" - це може бути, приміром, епідемія, стихійні лиха, катастрофи тощо.
+В разі оголошення надзвичайної ситуації влада має змогу організовувати санітарно-епідеміологічні заходи, проводити евакуацію, посилювати охорону громадського порядку, призупиняти роботу підприємств тощо.
+Ключова відмінність від надзвичайного стану - режим надзвичайної ситуації жодним чином не обмежує конституційні права і свободи людей.
+Натомість надзвичайний стан - це особливий правовий режим, за якого ці права можуть тимчасово обмежуватися - як-от свобода пересування, свобода зібрань тощо.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+UNIAN
+В Україні закривають всі тубдиспансери, хворі на туберкульоз кашляють на вулицях і заражають всіх навколо - такі побоювання висловлюють у соцмережах. Чи правда це і яка зараз ситуація із цією хворобою, дізналась ВВС News Україна.
+Перш ніж почути діагноз "туберкульоз" і почати приймати ліки, Тетяна Іванова пройшла всі кола пекла.
+Вісім місяців болю в усьому тілі і температури, сотні аналізів і оглядів.
+Так довго їй не могли поставити точний діагноз.
+На рентгені легені були чисті. У неї був туберкульоз лімфовузлів.
+Що треба знати про туберкульоз
+"Чому мій терапевт не відправила мене на ретельне обстеження на туберкульоз? Вона думала, що туберкульозом хворіють лише безхатьки, наркомани і люди з в'язниць? Туберкульоз - це ж не лише кашель", - говорить пані Іванова, яка працює в благодійній організації "Конвіктус Україна".
+За даними ВООЗ, в Україні щороку своєчасно не виявляють 23% випадків туберкульозу.
+Це є причиною його подальшого поширення.
+Що таке туберкульоз:
+інфекційне захворювання, викликане мікобакерією туберкульозу (МБТ, бацила Коха)
+передається повітряно-крапельним шляхом
+людина заражається, вдихаючи краплини вологи з паличкою МБТ, які виділив хворий при кашлі, чханні
+найчастіше вражає легені
+рідше - нирки або спинний мозок
+заразною є легенева, відкрита форма туберкульозу
+В січні 2020 року в Україні зареєстрували 2,4 тисячі нових хворих на туберкульоз. У лютому нових випадків було 2 000. А загалом від хвороби минулого місяця лікувались 20 тисяч людей.
+В 2018 році, за даними МОЗ, в Україні було 62,3 хворих на туберкульоз на 100 000 населення.
+У цей час у Польщі, за даними Світового банку, лише 16 хворих на сто тисяч наслення, у Білорусі - 31, у Словаччині - 6.
+Більше, ніж у нас, наприклад, хворих на туберкульоз було в Афганістані, Камбоджі, Гані.
+Чому все так погано?
+"Не вистачає сучасного обладнання, яке б дозволяло швидко діагностувати туберкульоз, люди не довіряють лікарям і не звертаються вчасно. Українці люблять займатися самолікуванням - антибіотики вільно продаються в аптеках, люди їх купують, не дотримуються схем лікування, кидають. Виникає проблема з поширенням резистентних штамів збудника", - перераховує причини Оксана Зінченко, кандидатка біологічних наук, доцент кафедри мікробіології, вірусології та біотехногії ОНУ імені І.І. Мечникова.
+Майже кожен четвертий випадок в Україні - це мультирезистентний туберкульоз (МРТБ). Тобто такий, що не піддається лікуванню протитуберкульозними препаратами першої лінії.
+За кількістю хворих із такою формою країна серед "світових лідерів", розповідає колишня очільниця МОЗ Уляна Супрун.
+Одна з причин, за її словами, - застаріла система протитуберкульозної допомоги, яка залишилась ще з часів СРСР. Складовою цієї системи є тривале лікування в диспансерах.
+"Коли ця система створювалася, не було ефективних ліків проти туберкульозу, тому пацієнтів розміщували у протитуберкульозні лікарні, диспансери або санаторії на тривалий час. Тепер такі ліки є, вони доступні в Україні, за пару тижнів їх прийому людина припиняє поширювати хворобу. Тривале перебування в стаціонарі та відсутність розділення хворих з різними формами туберкульозу збільшує ризик повторного зараження", - твердить пані Супрун.
+Що змінити?
+В Україні працює розгалужена система протитуберкульозних закладів: станом на 2018 рік було 68 тубдиспансерів, 21 туберкульозна лікарня для дорослих і дві для дітей. Всього понад 12 тисяч ліжок.
+Основні симптоми туберкульозу:
+кашель понад два тижні
+підвищена температура понад 7 днів
+ускладнене дихння
+біль у грудях
+поганий апетити, слабкість
+втрата ваги
+підвищена пітливість
+кровохаркання
+Тривалість лікування у таких закладах - від двох до трьох місяців. На них у 2018 році виділили 1 млрд 994 тисяч грн з бюджету. Для порівняння, на лікування інсультів — 539 млн грн.
+Змінити підходи до хворих намагалися задовго до Супрун. Програму реформування протитуберкульозних закладів Верховна Рада ухвалила ще у 2012 році. Повністю систему так і не змінили.
+В 2018 році провели "оптимізацію ліжкового фонду" тубдиспансерів. Тоді скоротили майже дві тисячі ліжок - 12,4%.
+В листопаді 2019 року уряд, який тоді очолював Олексій Гончарук, ухвалив нову концепцію розвитку системи протитуберкульозної допомоги.
+У ній йшлося про реорганізацію системи тубдиспансерів, їх злиття в один-два базові заклади на рівні області, де хворі можуть лікуватися у стаціонарі. Решту - перевести на амбулаторне у поліклініки і кабінети фтизіатрів.
+"Ліжка не лікують"
+В Україні немає жодного диспансеру, де б дотримувалися норм інфекційного контролю, говорить представник благодійної організації "100% ЖИТТЯ", лікар-інфекціоніст Віктор Третьяков.
+Ця організація минулого року супроводжувала понад 9 тисяч хворих на туберкульоз в Україні - волонтери підтримували хворих, привозили їм ліки і їжу.
+Сам пан Третьяков об'їздив багато тубдиспансерів. Він говорить, що у більшості з них умови жахливі, ремонти робили 30-40 років тому.
+Image caption
+Захворіти на туберкульоз можуть всі. Лише 20% серех хворих - це соціально незахищені верстви.
+Більшість хворих за два тижні лікування перестають бути заразними, їм не потрібно далі бути в стаціонарах, говорить Третьяков.
+"Якщо людина вже не виділяє паличку, то і немає потреби. А якщо людей дуже довго тримати в стаціонарі, вони заражають один одного. Наприклад, там лікується вже знебацилена людина, а поступає хтось, хто виділяє бактерії. Так з'являються резистентні форми хвороби", - пояснює лікар.
+Лікування у тубдиспансерах і туберкульозна лікарнях може тривати до 100 днів.
+Що може допомогти в боротьбі з туберкульозом?
+раннє виявлення - скринінг-опитування
+бактеріологічні та генетичні методи діагностики
+призначення схеми лікування тільки у відповідності до профілю чутливості мікобактерії
+амбулаторне лікування, госпіталізація - при поганому фізичному стані людини
+точне виконання режиму прийому препаратів та тривалості лікування
+соціальний та психологічний супровід пацієнта, забезпечення прихильності до лікування, захист прав пацієнта
+обстеження контактних осіб
+інформаційна робота, зниження стигми та дискримінації
+Партнерство "Зупинимо туберкульоз. Україна"
+"Ліжка не лікують туберкульоз, і госпіталізація хворого "в ліжко" не пов'язана з ефективністю його лікування", - підтримує реформу ТБ галузі Наталія Гранкіна, медична директорка Дніпропетровської обласної фтізіатрії.
+За її словами, туберкульоз можна лікувати амбулаторно, використовуючи міжнародні підходи, наприклад, новітні протитуберкульозні препарати, які дозволяють вилікувати резистентні форми за 9-12 місяців замість 24-36 місяців у ліжку.
+При цьому хворий не зобов'язаний весь цей час перебувати у стаціонарі. Пані Гранкіна розповідає про лікування на Дніпровщини хворих за допомогою інтерактивних дистанційних методів - хворий щодня надсилає відео своєму лікарю.
+Вона також відверто говорить, що часто стаціонарні заклади не відповідають міжнародним стандартам.
+Протитуберкульозні диспансери повинні мати споруди, які очищають і видають назовні чисту знезаражену воду.
+"Очисні споруди у нас є лише в обласному протитуберкульозному диспансері. У місті Павлоград Дніпропетровської області, наприклад, таких споруд немає. Більш того, ми мали немалу кількість проблем із павлоградським водоканалом щодо стічних вод".
+Павлоградський протитуберкульозний диспансер розташований на околиці міста. Зовні це звичайна пострадянська будівля, яких так багато у маленьких містечка: три поверхи, сіра цегла, дерев'яні вікна, давній ремонт, меблі ще з часів СРСР.
+Цей тубдиспансер обслуговвав місто Павлоград, а також весь Павлоградський та Межівський райони.
+Раніше у ньому стаціонарно лікували хворих на туберкульоз, тепер тут лише поліклініка, куди можна прийти на консультації. Якщо треба в лікарню - хворих відправляють у Кривий ріг чи Дніпро.
+"Як тепер лікуватимуться пацієнти із відкритою формою? Як можна проконтролювати лікування?", - обурюється лікарка-фтизіатр Тетяна Шишкіна, яка працювала у Павлоградському тубдиспансері.
+Вона категорично проти закриття таких закладів.
+Image caption
+Павлоградський протитуберкульозний диспансер
+За її словами, за останні три роки сюди до стаціонарних відділень госпіталізували 919 хворих із відкритою формою, з них 543 - це люди, що мали стійку форму туберкульозу, яку лікують довго і яку потрібно контролювати.
+"Одна людина із відкритою формою, якщо вона не проходить лікування, може заражати до 15 людей. Тобто уявіть потенційне число заражених! Якщо заклад закриватимуть, то ми можемо говорити про можливий початок епідемії в місті", - обурюється пані Шишкіна.
+Хворих не виганятимуть на вулицю, стаціонар працює далі, але ліжка будуть максимально сконцентровані на базі обласного Дніпропетровського протитуберкульозного диспансеру і диспансеру Кривого Рогу, відповідає пані Гранкіна.
+Згідно з реформою, у кожній області має залишитись мінімум один великий заклад — фтизіатричний центр або центр легеневих хвороб, де можна лікуватися на стаціонарі.
+Головне, щоб ці заклади розміщувалися не на далекій відстані й хворі могли до них доїхати, говорить пан Третьяков з "100% ЖИТТЯ".
+Хто може захворіти:
+всі
+але група ризику - діти і літні, люди з ослабленим імунітетом
+люди з хронічними захворюваннями
+ВІЛ-інфіковані
+люди, які перебувають у контакті з хворими
+Також продовжать роботу кабінети фтізіатрів у районах, де пацієнти зможуть отримувати ліки. Крім того, у планах уряду - ввести посади міжрайонних фтизіатрів у регіональних центрах.
+Директорка Дніпропетровської фтізіатрії говорить, що амбулаторна служба працюватиме в області й надалі, і саме ці фтизіатри будуть відповідати за виявленням хворих.
+Але реформа лікування туберкульозу, як і вся медреформа, може опинитися під питанням через зміну керівництва МОЗ і ситуацію з коронавірусом.
+Лікар-інфекціоніст Віктор Третьяков пояснює: коронавірус може погіршити ситуацію з туберкульозом тому, що потенційно хворі на ТБ - якраз у групі ризику.
+"Це може збільшити смертність", - говорить лікар.
+Стигма
+Боротьба Тетяни Іванової з хворобою тривала два роки і три місяці.
+Зараз вона видужала і тепер розповідає про свій досвід, виступає на тренінгах і семінарах, присвячених туберкульозу, закликає долати стигму довкола цієї хвороби.
+"Один з важливих пунктів лікування від туберкульозу - не боятися говорити. Я думала, що ця хвороба - це все, це вирок. Але це ж не так", - каже Тетяна Іванова під час свого виступу на тренінгу організації "Зупинимо туберкульоз. Україна".
+В Україні, яка серед лідерів у Європі з поширення туберкульозу, навколо цієї хвороби справді багато міфів, неперевіреної інформації та страхів.
+"Чому ж, коли є ефективні ліки, в Україні так багато хворих? Для багатьох людей страшно визнати, що у тебе туберкульоз. Страшно піти лікуватись. Страшно відчувати себе відчуженим, - говорить лікарка Гунта Дравніце, голова проєкт "Підтримка зусиль у протидії туберкульозу в Україні", - Туберкульоз - виліковний. Це варто пам'ятати".
+За участю позаштатного кореспондента ВВС News Україна Артема Лисенка
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Коронавірус: Китай починає послаблювати карантин</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+Image caption
+Ухань закритий від середини січня цього року
+Від півночі вівторка у китайській провінції Хубей, звідки новий коронавірус поширився світом, знімають обмеження на пересування для здорових місцевих жителів.
+Разом із тим, карантин у місті Ухань, де, власне, і почався перший спалах хвороби, буде частково скасовано лише 8 квітня.
+24 березня в Ухані зареєстрували лише один новий випадок захворювання на COVID-19. Проте у попередні п'ять днів нових випадків зараження взагалі не було.
+Як перевести на віддалену роботу всю країну
+У решті ж світу, навпаки, посилюють карантині заходи та обмеження. Всесвітня організація з охорони здоров'я вважає, що пандемія коронавірусу в світі і надалі розростається.
+Ухань був закритим від решти світу від середини січня цього року. Проте зараз представники китайської влади заявили, що всі, хто мають так званий "зелений код" на розповсюдженому телефонному додатку, зможуть виїхати з міста з 8 квітня.
+За офіційними даними, впродовж останніх 24 годин у Китаї зафіксували 78 нових випадків захворювання. За винятком чотирьох, усі вони стосуються людей, які повернулися з-за кордону.
+Ця так звана "друга хвиля" імпортованого зараження також спостерігається у Південній Кореї та Сингапурі, які до цього успішно зупинили поширення хвороби всередині країни впродовж тижнів.
+Південна Корея заявила про найменшу кількість нових інфікованих від 29 лютого.
+Коронавірус у Південній Кореї йде на спад: як їм це вдалося?
+Китай готується відновлювати свою репутацію
+Робін Брант, BBC News, Шанхай
+Китай вважає себе вже майже "посткоронавірусною" країною.
+Впродовж останнього тижня лікарі з Уханя роздають рекомендації іншим країнам по всьому світу: що робити, щоб захистити "першу лінію оборони" медичних працівників, які помилки були зроблені в Китаї, зокрема, і надання допомоги хворим без відповідного захисного одягу, як це було у перші дні поширення хвороби в Китаї.
+Новини про те, що кількість смертей в Італії перевищила кількість смертей в Китаї, місцеві медіа висвітлювали ледь не з тріумфальними нотками.
+У той таки час зберігається паніка щодо загрози "другої хвилі" випадків захворювання, "імпортованих" тими, хто прибуває з-за кордону. Це підживлює і ще одну поширену думку - правильну чи ні, - що деякі країни не сприймають загрозу серйозно, бо не роблять тих самих кроків, до яких вдався Китай, аби зупинити поширення хвороби.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Коронавірус: чи можна ним заразитися двічі?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+Image caption
+Вчені з усього світу вивчають коронавірус
+Деякі пацієнти одужали від Covid-19, їхні тести на коронавірус були негативні, але згодом знову стали позитивними. Інфікування коронавірусами, як і звичайна застуда, зазвичай виробляє у пацієнтів імунітет. То чим відрізняється цей вірус?
+Одним із перших, хто неприємно здивував лікарів, став чоловік за 70.
+Чи правда, що молодь хворіє на коронавірус в легкій формі
+Системи штучної вентиляції легень. Що це і чи справді їх бракує
+Ходити в храм чи ні: що каже церква про карантин
+Бебі-бум чи хвиля розлучень? До чого приведе карантин
+У лютому йому діагностували коронавірус і помістили в ізоляцію в токійській лікарні.
+За даними японського телеканалу NHK, він одужав і повернувся до звичного життя, навіть їздив громадським транспортом. Але за кілька днів він знову занедужав, у чоловіка піднялась температура.
+Він повернувся до лікарні, де здивував себе і лікарів позитивним тестом на вірус.
+Копирайт изображения
+GETTY IMAGES
+Image caption
+Уряд Британії вибудував свою стратегію боротьби з Covid-19 на концепції вироблення колективного імунітету серед населення
+І це - не єдиний подібний випадок в Японії. Чому так відбувається?
+Вірусний відскок
+Луїс Енхуанес, вірусолог в Іспанському національному центрі біотехнологій (CSIC), розповів BBC, що принаймні 14% пацієнтів, які після лікування отримали негативний тест Covid-19, за деякий час знову мали позитивні результати.
+Він вважає, що це не повторне інфікування, а випадки "відскоку" вірусу.
+"Моє пояснення, серед багатьох інших можливих, полягає у тому, що загалом цей коронавірус імунізує населення, але імунна відповідь не дуже сильна (у деяких людей. - Ред.)", - говорить Енхуанес.
+"Коли ця імунна реакція сповільнюється, вірус, який залишається в якомусь резервуарі в організмі, повертається назад", - додає вірусолог.
+Вірус може лишитися в організмі
+Деякі віруси можуть залишатися в організмі три місяці або довше.
+Копирайт изображения
+GETTY IMAGES
+Image caption
+За даними експертів, 14% пацієнтів з негативними тестами на Covid-19 пізніше знову мали позитивні результати
+"Коли людина отримує позитивний тест на вірус, а згодом має негативний тест, ми припускаємо, що у неї виробився імунітет, тому вірус не має з'явитися повторно", - каже Енхуанес.
+"Але деякі інфекційні агенти можуть лишатися у тканинах організму, на які не поширилась захисна реакція організму - наприклад, у інших органах", - додає він.
+Але у Covid-19 є дещо, що інтригує науковців, - це короткий період між одужанням та повторним позитивним тестом.
+Такі різні віруси
+Ми знаємо, що імунітет працює по-різному при різних захворюваннях.
+У випадку кору одноразової вакцинації у дитинстві зазвичай достатньо, щоб забезпечити людині довічний імунітет. Однак деякі органи охорони здоров'я рекомендують людям певного віку повторну вакцинацію більш сучасною вакциною.
+Як коронавірус шириться планетою. Мапа
+Коронавірус: що треба знати
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Є й інші віруси, проти яких вакцини не настільки ефективні, тому від них потрібно ревакцинуватися через регулярні проміжки часу.
+А є вакцини, наприклад, проти грипу, які потрібно робити щороку, оскільки віруси мутують.
+Намагаються зрозуміти
+Але оскільки Covid-19 - це новий вірус, вчені досі намагаються зрозуміти, чим пояснити такий короткий проміжок часу до повторного прояву інфекції.
+Ісідоро Мартінес, науковий співробітник Інституту здоров'я Карлоса III в Мадриді, каже, що хоча повторне інфікування коронавірусом трапляється, дивно, що у випадку Covid-19 це відбувається настільки швидко після негативних тестів.
+Копирайт изображения
+GETTY IMAGES
+"Якщо не буде стійкого імунітету, в наступні епідемії, протягом одного-двох років, ви зможете заразитися повторно. Це нормально, - розповів Мартінес BBC.
+"Але дуже рідко людина повторно заражається тим самим вірусом після одужання. Також, наскільки нам відомо, цей коронавірус мутує не так сильно, як вірус грипу", - додав він.
+Тимчасовий сплеск
+Його пояснення схоже на думку Луїса Енхуанеса.
+"Можливо, люди, які знову мають позитивні тести на Covid-19 після негативного тестування, переживають тимчасовий сплеск інфекції, перш ніж вона остаточно зникне".
+Але обидва дослідники застерігають, що для розуміння природи Covid-19 потрібні подальші дослідження.
+У Панамериканській організації охорони здоров'я (PAHO) розповіли BBC, що "Covid-19 - це новий вірус, про який ми з кожним днем дізнаємось більше", тому не можна з певністю пояснити випадки повторного зараження.
+Але науковці намагаються знайти відповідь, щоб допомогти урядам вирішити, які заходи вживати.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Коронавірус у Південній Кореї йде на спад: як їм це вдалося?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+EPA
+Image caption
+Мешканці Сеула дезінфікують свої райони
+Південна Корея повідомила про найменшу кількість нових випадків коронавірусу з моменту, коли рівень зараження досяг піку чотири тижні тому. Це дає надію, що спалах у найбільш ураженій країні Азії після Китаю може піти на спад.
+За останню добу в країні зафіксували 64 нові випадки Covid-19, загалом їх - 8 961, з яких 111 смертельних.
+Однак чиновники охорони здоров'я застерігають, що радіти зарано - за їхніми словами, на країну все ще чекає довга війна з інфекцією.
+Закриті ринки і заборонені пробіжки: в італійській Ломбардії ще посилюють карантин
+Надія є: п'ять причин порадіти під час пандемії коронавірусу
+Відповіді на головні питання про коронавірус
+Наразі центром пандемії є Європа.
+Італія повідомила про 651 смерть у неділю, загальна кількість загиблих у країні склала 5 476. В Іспанії зафіксували 394 нових смертей, загалом від коронавірусу там загинули 1 720 людей.
+Водночас мер Нью-Йорка попередив про погіршення ситуації, зокрема через брак основних медичних товарів.
+Очікування, що боротьба з вірусом буде тривалою, підкріпили новини з Японії - прем'єр-міністр країни вперше визнав, що Олімпійські ігри 2020 року в Токіо можуть перенести.
+У чому секрет успіху Південної Кореї?
+Щодня у Південній Кореї на коронавірус тестують майже 20 тис. людей - це найбільша кількість тестів на душу населення у світі.
+У країні створили мережу державних та приватних лабораторій та десятки мобільних центрів, де люди із симптомами можуть перевірити стан здоров'я.
+Південна Корея розробила свій підхід після спалаху Близькосхідного респіраторного синдрому (MERS) у 2015 році, коли в країні була найбільша кількість хворих після Саудівської Аравії, а 36 людей померли.
+MERS змусив країну переосмислити свій підхід до інфекційних захворювань, і Центри контролю за хворобами створили спеціальну комісію для підготовки до найгіршого сценарію - і цей крок, схоже, цілком себе виправдав.
+Як коронавірус шириться планетою. Мапа
+Коронавірус: що треба знати
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Суттєво змінилися закони щодо управління та публічного обміну інформацією про пацієнтів із інфекційними захворюваннями, і їхню дію можна було побачити цього року, коли уряд відправляв людям на мобільні повідомлення, щоб вони знали, що перебувають поблизу хворої людини.
+Цими вихідними уряд посилив превентивні дії, надсилаючи попередження про надзвичайні ситуації, закликаючи людей триматися подалі від місць скупчення людей, таких як церкви, караоке, нічні клуби та тренажерні зали.
+Релігійних лідерів закликали перевіряти температуру вірян і під час служб зберігати дистанцію між ними не менше двох метрів.
+Деяким церквам за порушення цих правил наразі загрожують судові позови.
+Чому в країні бояться нової хвилі?
+Як повідомляє інформаційна агенція Yonhap, у країні було дві хвилі інфекції - перша почалася 20 січня з першого підтвердженого випадку, а друга - з масового інфікування у релігійній спільноті.
+Копирайт изображения
+EPA
+Image caption
+Пасажирів, які прибули до Інчхона з Лондона, відправляють на двотижневий карантин
+Зараз є побоювання, що ініціювати третю хвилю можуть інфіковані з-за кордону.
+Уряд планує встановити близько 20 тестувальних кабінок в аеропорту Інчхона, щоб пришвидшити процес тестування усіх прибулих з Європи.
+Нові процедури в'їзду почали діяти у неділю. Наразі до країни приїхали 152 людини із симптомами вірусу, які чекають на результати тестів.
+Аналіз
+Лора Бікер, кореспондент ВВС у Сеулі
+Південна Корея перебуває у критичній точці. Так, агресивне використання технології для відстеження вірусу та масове тестування усіх, хто контактував з інфікованими, - стратегія, яка виявилася успішною. Але лікарі по всій країні запитують - що далі?
+Мета - відкрити школи через два тижні. Саме тому уряд надсилає термінові повідомлення, закликаючи населення протягом наступних 15 днів дотримуватися соціальної дистанції, щоб уникнути сплеску інфекцій. Прийшла весна, і люди прагнуть насолодитися теплом. Почуття солідарності й того, що це битва, яку потрібно виграти разом, поступово розмивається. Служби охорони здоров'я сподіваються, що суворе попередження про те, що ця війна досі триває, змусить людей утримуватись від масових зібрань.
+Тим часом лікарі обговорюють наступні можливі кроки. Підхід "відстеження, тестування, лікування" будуть застосовувати й надалі. Але його також потрібно буде продумати. Наприклад, що робити, якщо інфекція потрапить до шкільного класу? Закривати цілу школу? Знову закрити всі школи? І далі порушувати нормальне життя?
+На пресконференції голова Національного медичного комітету д-р О Мюн-дон заявив журналістам, що після відкриття шкіл може бути ще один сплеск. Його також турбує можлива повторна активація вірусу наступної зими. Він згадав, що, можливо, прийшов час дозволити частині населення захворіти. Це - так звана теорія "колективного імунітету". Чиновник визнає ризик, але також вважає, що зараз саме час вести ці розмови та попередити громадськість.
+Парадокс успіху Південної Кореї полягає в тому, що після тривалої самовідданої боротьби з вірусом, медики в країні мають продовжувати працювати. Це трохи схоже на підйом на круту гору, коли не знаєш, скільки лишилось до вершини або які перешкоди можуть бути на шляху. Жахлива ситуація в Європі змушує місцеву владу боятися, що якщо вони трохи розслабляться, на них може чекати така сама доля.
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Бебі-бум чи розлучення? Що буде після карантину. Огляд ЗМІ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Копирайт изображения
+GETTY IMAGES
+У вівторок, 24 березня, в огляді преси читайте про таке.
+Чи буде бебі-бум через вірус
+Теплий вологий клімат пригнічує вірус
+Американка розповідає, що через коронавірус втратила слух, нюх і смак
+Чому так багато людей померло від коронавірусу в Італії
+Розлучення через COVID-19
+Пандемія коронавірусу навряд чи приведе до бебі-буму, однак може збільшити кількість розлучень, пише журналістка Петула Дворжак у колонці для Washington Post.
+Адже карантин та дистанційна робота дають змогу партнерам побачити один одного у незвичному режимі.
+Авторка зізнається, що запровадила разом з чоловіком певні правила життя на час карантину.
+Чи можна займатися сексом під час коронавірусу?
+Як перевіритися на коронавірус?
+"Коли я розмовляю телефоном з жертвами насильства, йому не дозволено в мене питати, де лежить сир, гірчиця чи будь-що інше, - пише журналістка. - Я нагадую йому надягати сорочку для відеоконференцій, а він тримає вдома собак, коли я зачиняюся в машині на час телефонних інтерв'ю".
+"Якщо ми зможемо пережити ці правила, ми переживемо все", - вважає авторка.
+Топовий британський адвокат з розлучень Фіона Шеклтон, яка вела розлучні процеси Пола Маккартні, Мадонни та інших знаменитостей, також очікує на бум у своєму бізнесі. Про це вона сказала на засіданні британського парламенту.
+"Пік зазвичай припадає на літні канікули та Різдво, коли люди багато часу проводять разом, - сказала вона. - Уявіть, що буде, коли сім'ї зачинені вдома дуже довгий час".
+Однак все може бути і не так погано, якщо вірити спортивному кореспонденту Марку Зінно зі штату Меріленд. За його словами, віддалена робота дозволяє вам побачити, наскільки важлива робота вашого партнера і як старанно він чи вона працює.
+"Ви про це ніколи не дізнаєтесь, доки не сядете з ними поруч і не побачите їх у процесі", - наголошує Зінно.
+Клімат проти коронавірусу
+Копирайт изображения
+GETTY IMAGES
+Потепління і висока вологість суттєво знижують поширення COVID-19, пише Daily Mail, посилаючись на дослідження китайських учених.
+Дослідники проаналізували темпи зараження коронавірусом за тривалий час у 100 китайських містах, де понад 40 людей заразилися у період із 21 по 23 січня.
+Вони побачили, що коли температура повітря підвищилася з мінус 20 до плюс 20 градусів за Цельсієм, середня кількість людей, яким передала вірус заражена людина, зменшилася з 2,5 до 1,5.
+Так само, чим більша була вологість, тим менші темпи зараження.
+Як порожніють вулиці через коронавірус. Фото
+Коронавірус. Відповідаємо на поширені запитання
+Учені внесли поправку на густоту населеності під час складання графіку.
+Раніше вважалося, що носій вірусу заражає ним від 2 до 2,5 людей.
+Китайські вчені також показали, що вірус повільніше поширюється у вологому, тропічному кліматі на кшталт малайзійського або таїландського, а швидше - у сухішому та холоднішому, як в Ірані, Японії та Кореї.
+Ученим достеменно невідомо, чому віруси краще передаються і виживають на холоді. Однак ми знаємо, що взимку людський імунітет пригнічується, а холодне та сухе повітря висушує слизову оболонку носа, що є першим рівнем захисту від мікроорганізмів.
+Як коронавірус шириться планетою. Мапа
+Як подорожувати під час епідемії
+Як перевіритися на коронавірус?
+Чи захищають медичні маски від вірусу?
+Втратила слух через коронавірус?
+Копирайт изображения
+GETTY IMAGES
+Двадцятирічна американська студентка Джулія Бускаглія не хотіла робити тест на COVID-19 після повернення з Італії у березні, адже в неї не було всіх типових для цієї хвороби симптомів.
+Джулія з Нью-Йорку відвідала Флоренцію в січні, пише Daily Mail.
+А 29 лютого прокинулася з головним болем, температурою та болем у горлі, пише вона в своєму Twitter. Коли відвідала лікаря наступного дня, почала втрачати слух у лівому вусі, але лікар сказав, що в неї застуда.
+Знаменитості, які підхопили коронавірус
+Депутат Шахов захворів на коронавірус
+Уже 3 березня, каже Джулія, вона втратила слух, нюх та смак, однак в неї не було характерного для коронавірусу сухого кашлю. Нежиті також не було. Дівчина лікувалася протизапальним засобом Tylenol.
+Після повернення до Сполучених Штатів 5 березня вона самоізолювалася, хоча ніхто не питав у неї на митному контролі, яку країну вона відвідувала.
+Лише 14 березня за наполяганням батьків Джулія зробила тест на COVID-19, який дав позитивний результат. Довелося кілька разів проситися зробити тест, адже їй спочатку відмовляли.
+На момент отримання результатів у дівчини досі не було кашлю.
+Джулія каже, що повністю вилікувалася, однак застерігає, що "нам повідомляють не про всі симптоми", а також, що "не треба мати всі симптоми, щоб мати вірус".
+Особливості Італії
+Копирайт изображения
+GETTY IMAGES
+Велика кількість фатальних випадків коронавірусної хвороби в Італії пояснюється демографією і способом рахування випадків, пише Telegraph.
+Ця країна вже обігнала Китай за кількістю смертей від коронавірусу.
+Італія - друга за старістю населення країна в світі. Середній вік пацієнтів там - 67 років, а в Китаї - 46, каже науковий радник італійського міністра охорони здоров'я, професор Вальтер Річіарді.
+Дослідження показали, що 87% смертей в Італії припадало на людей, старших за 70.
+Інша причина полягає в тому, що всі італійські пацієнти, які мали коронавірус і померли, вважаються такими, що померли від коронавірусу, навіть якщо в них були інші хвороби.
+Коронавірус: в Італії померла рекордна кількість людей
+"Ніхто не знає, що буде завтра". Що кажуть про карантин українці в Італії
+"Наше дослідження Національного Інституту Здоров'я показало, що лише 12% сертифікатів про смерть свідчать, що смерть спричинена коронавірусом, а 88% пацієнтів померли від хвороби, яку мали до того, а часто таких було дві чи три", - каже Річіарді.
+Це не означає, що коронавірус не мав впливу на смерть цих пацієнтів, але демонструє, що велика смертність в Італії пояснюється тим, що в більшості пацієнтів були інші проблеми зі здоров'ям, пише видання.
+Експерти також виділяють інші фактори, зокрема, популярність куріння та забруднення повітря в Італії.
+Через останній фактор особливо потерпає регіон Ломбардія, де спостерігають найбільший спалах коронавірусу в країні.
+За словами професора Лондонської школи гігієни і тропічної медицини Мартіна Маккі, рано порівнювати країни Європи за рівнем захворюваності, адже невідомо, скільки є випадків із помірними симптомами.
+Огляд підготувала Маргарита Малюкова, Служба Моніторингу BBC
+Хочете отримувати найважливіші новини в месенджер? Підписуйтеся на наш Telegram або Viber!
+</t>
   </si>
 </sst>
 </file>
@@ -5760,15 +6873,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F146"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G90" activeCellId="0" sqref="G90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C148" activeCellId="0" sqref="C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7808,7 +8923,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="431.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="n">
         <v>113</v>
       </c>
@@ -7825,7 +8940,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="431.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="n">
         <v>114</v>
       </c>
@@ -7842,7 +8957,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="431.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="n">
         <v>115</v>
       </c>
@@ -7859,7 +8974,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="431.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="n">
         <v>116</v>
       </c>
@@ -7879,7 +8994,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="431.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="n">
         <v>117</v>
       </c>
@@ -7896,7 +9011,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="431.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="n">
         <v>118</v>
       </c>
@@ -7913,7 +9028,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="431.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="n">
         <v>119</v>
       </c>
@@ -7928,6 +9043,452 @@
       </c>
       <c r="F121" s="2" t="s">
         <v>296</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E122" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E123" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E124" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D125" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E125" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D126" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E126" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="D127" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E127" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D128" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E128" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D129" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E129" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="D130" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E130" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D131" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E131" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D132" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E132" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D133" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E133" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D134" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E134" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C135" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="D135" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E135" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D136" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E136" s="0" t="s">
+        <v>340</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D137" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E137" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D138" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E138" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C139" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D139" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E139" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B140" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D140" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E140" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C141" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="D141" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E141" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D142" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E142" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D143" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E143" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C144" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="D144" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E144" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D145" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E145" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B146" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="D146" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E146" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>